<commit_message>
1. requirements updated 2.pivot table example added 3.word clouds 4. covid random analysis
</commit_message>
<xml_diff>
--- a/class1_explore/scrapers/covid_wiki_stats.xlsx
+++ b/class1_explore/scrapers/covid_wiki_stats.xlsx
@@ -498,17 +498,17 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>17,039,160</t>
+          <t>17,109,335</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>667,084</t>
+          <t>668,801</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>9,964,678</t>
+          <t>10,000,738</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -529,17 +529,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4511890</t>
+          <t>4543362</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>153045</t>
+          <t>153769</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2211365</t>
+          <t>2216659</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -560,12 +560,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2556207</t>
+          <t>2556765</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>90212</t>
+          <t>90383</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -746,17 +746,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>351575</t>
+          <t>353536</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>9278</t>
+          <t>9377</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>324557</t>
+          <t>326628</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -772,27 +772,27 @@
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Iran</t>
+          <t>United Kingdom[j]</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>301530</t>
+          <t>302301</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>16569</t>
+          <t>45999</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>261200</t>
+          <t>No data</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>[26]</t>
+          <t>[27]</t>
         </is>
       </c>
     </row>
@@ -803,27 +803,27 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>United Kingdom[j]</t>
+          <t>Iran</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>301455</t>
+          <t>301530</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>45961</t>
+          <t>16569</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>No data</t>
+          <t>261200</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>[28][29]</t>
+          <t>[28]</t>
         </is>
       </c>
     </row>
@@ -839,12 +839,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>282641</t>
+          <t>285430</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>28441</t>
+          <t>28443</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -854,7 +854,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>[30]</t>
+          <t>[29]</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>[31]</t>
+          <t>[30]</t>
         </is>
       </c>
     </row>
@@ -916,7 +916,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>[32]</t>
+          <t>[31]</t>
         </is>
       </c>
     </row>
@@ -932,22 +932,22 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>272590</t>
+          <t>274219</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2816</t>
+          <t>2842</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>228569</t>
+          <t>231198</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>[33]</t>
+          <t>[32]</t>
         </is>
       </c>
     </row>
@@ -963,22 +963,22 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>246776</t>
+          <t>247158</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>35129</t>
+          <t>35132</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>199031</t>
+          <t>199796</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>[34][35]</t>
+          <t>[33][34]</t>
         </is>
       </c>
     </row>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>[36]</t>
+          <t>[35]</t>
         </is>
       </c>
     </row>
@@ -1025,22 +1025,22 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>228924</t>
+          <t>229891</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>5659</t>
+          <t>5674</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>212557</t>
+          <t>213539</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>[37]</t>
+          <t>[36]</t>
         </is>
       </c>
     </row>
@@ -1056,22 +1056,22 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>209089</t>
+          <t>209321</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>9214</t>
+          <t>9217</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>191325</t>
+          <t>191781</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>[39][38]</t>
+          <t>[38][37]</t>
         </is>
       </c>
     </row>
@@ -1087,22 +1087,22 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>185196</t>
+          <t>186573</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>30238</t>
+          <t>30254</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>81311</t>
+          <t>81500</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>[40]</t>
+          <t>[39]</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>[42][43]</t>
+          <t>[41][42]</t>
         </is>
       </c>
     </row>
@@ -1149,22 +1149,22 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>118300</t>
+          <t>121263</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4603</t>
+          <t>4671</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>83461</t>
+          <t>85546</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>[44]</t>
+          <t>[43]</t>
         </is>
       </c>
     </row>
@@ -1180,22 +1180,22 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>115470</t>
+          <t>115619</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>8917</t>
+          <t>8923</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>100465</t>
+          <t>100631</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>[47]</t>
+          <t>[46]</t>
         </is>
       </c>
     </row>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>[48]</t>
+          <t>[47]</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>[49]</t>
+          <t>[48]</t>
         </is>
       </c>
     </row>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>[50]</t>
+          <t>[49]</t>
         </is>
       </c>
     </row>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>[51][52][53]</t>
+          <t>[50][51]</t>
         </is>
       </c>
     </row>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>[54]</t>
+          <t>[52]</t>
         </is>
       </c>
     </row>
@@ -1361,27 +1361,27 @@
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>China[q]</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>84165</t>
+          <t>84370</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4634</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>78957</t>
+          <t>35824</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>[55]</t>
+          <t>[53][54]</t>
         </is>
       </c>
     </row>
@@ -1392,27 +1392,27 @@
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>China[q]</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>83193</t>
+          <t>84165</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>5623</t>
+          <t>4634</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>35572</t>
+          <t>78957</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>[56][57]</t>
+          <t>[55]</t>
         </is>
       </c>
     </row>
@@ -1428,12 +1428,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>79782</t>
+          <t>80100</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>5730</t>
+          <t>5739</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>[58]</t>
+          <t>[56]</t>
         </is>
       </c>
     </row>
@@ -1474,7 +1474,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>[59]</t>
+          <t>[57]</t>
         </is>
       </c>
     </row>
@@ -1505,7 +1505,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>[60]</t>
+          <t>[58]</t>
         </is>
       </c>
     </row>
@@ -1516,27 +1516,27 @@
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Ukraine[r]</t>
+          <t>Israel[r]</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>68794</t>
+          <t>69603</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1673</t>
+          <t>499</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>38154</t>
+          <t>43776</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>[61]</t>
+          <t>[59]</t>
         </is>
       </c>
     </row>
@@ -1547,27 +1547,27 @@
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Israel[s]</t>
+          <t>Ukraine[s]</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>68299</t>
+          <t>68794</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>491</t>
+          <t>1673</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>32746</t>
+          <t>38154</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>[62]</t>
+          <t>[60]</t>
         </is>
       </c>
     </row>
@@ -1583,22 +1583,22 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>67518</t>
+          <t>67665</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>548</t>
+          <t>553</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>61442</t>
+          <t>61765</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>[63]</t>
+          <t>[61]</t>
         </is>
       </c>
     </row>
@@ -1614,22 +1614,22 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>66662</t>
+          <t>67335</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>9833</t>
+          <t>9836</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>18163</t>
+          <t>18196</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>[65]</t>
+          <t>[63]</t>
         </is>
       </c>
     </row>
@@ -1640,27 +1640,27 @@
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Dominican Republic</t>
+          <t>Kuwait</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>66182</t>
+          <t>66529</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1123</t>
+          <t>445</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>33947</t>
+          <t>57330</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>[66]</t>
+          <t>[64]</t>
         </is>
       </c>
     </row>
@@ -1671,27 +1671,27 @@
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Kuwait</t>
+          <t>Dominican Republic</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>65903</t>
+          <t>66182</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>444</t>
+          <t>1123</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>56467</t>
+          <t>33947</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>[67]</t>
+          <t>[65]</t>
         </is>
       </c>
     </row>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>[68][69]</t>
+          <t>[66][67]</t>
         </is>
       </c>
     </row>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>[70]</t>
+          <t>[68]</t>
         </is>
       </c>
     </row>
@@ -1784,7 +1784,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>[72]</t>
+          <t>[70]</t>
         </is>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>[73][74]</t>
+          <t>[71][72]</t>
         </is>
       </c>
     </row>
@@ -1831,22 +1831,22 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>50613</t>
+          <t>50868</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1725</t>
+          <t>1727</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>35875</t>
+          <t>36140</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>[75]</t>
+          <t>[73]</t>
         </is>
       </c>
     </row>
@@ -1877,7 +1877,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>[76]</t>
+          <t>[74]</t>
         </is>
       </c>
     </row>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>[77]</t>
+          <t>[75]</t>
         </is>
       </c>
     </row>
@@ -1939,7 +1939,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>[78][79]</t>
+          <t>[76][77]</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>[80]</t>
+          <t>[78]</t>
         </is>
       </c>
     </row>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>[81][82]</t>
+          <t>[79][80]</t>
         </is>
       </c>
     </row>
@@ -2032,7 +2032,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>[83]</t>
+          <t>[81]</t>
         </is>
       </c>
     </row>
@@ -2063,7 +2063,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>[84]</t>
+          <t>[82]</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>36471</t>
+          <t>36541</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2089,12 +2089,12 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>25389</t>
+          <t>25471</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>[85]</t>
+          <t>[83]</t>
         </is>
       </c>
     </row>
@@ -2105,27 +2105,27 @@
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Ghana</t>
+          <t>Kyrgyzstan</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>35142</t>
+          <t>35143</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>1364</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>31286</t>
+          <t>24474</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>[86]</t>
+          <t>[84]</t>
         </is>
       </c>
     </row>
@@ -2136,27 +2136,27 @@
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Switzerland[v]</t>
+          <t>Ghana</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>34802</t>
+          <t>35142</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1703</t>
+          <t>175</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>31100</t>
+          <t>31286</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>[87][88]</t>
+          <t>[85]</t>
         </is>
       </c>
     </row>
@@ -2167,27 +2167,27 @@
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Kyrgyzstan</t>
+          <t>Switzerland[v]</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>34592</t>
+          <t>35022</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1347</t>
+          <t>1704</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>22296</t>
+          <t>31100</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>[89]</t>
+          <t>[86][87]</t>
         </is>
       </c>
     </row>
@@ -2203,22 +2203,22 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>31901</t>
+          <t>33049</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1001</t>
+          <t>1004</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>23507</t>
+          <t>24179</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>[90]</t>
+          <t>[88]</t>
         </is>
       </c>
     </row>
@@ -2234,22 +2234,22 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>31211</t>
+          <t>31560</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>438</t>
+          <t>441</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>24495</t>
+          <t>25168</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>[91]</t>
+          <t>[89]</t>
         </is>
       </c>
     </row>
@@ -2265,22 +2265,22 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>29229</t>
+          <t>29831</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1186</t>
+          <t>1200</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>19592</t>
+          <t>20082</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>[92][93]</t>
+          <t>[90][91]</t>
         </is>
       </c>
     </row>
@@ -2291,27 +2291,27 @@
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Ireland[y]</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>25942</t>
+          <t>26027</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1764</t>
+          <t>1763</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>23932</t>
+          <t>24000</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>[94]</t>
+          <t>[92]</t>
         </is>
       </c>
     </row>
@@ -2322,7 +2322,7 @@
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Serbia[y]</t>
+          <t>Serbia[z]</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>[95]</t>
+          <t>[93]</t>
         </is>
       </c>
     </row>
@@ -2353,7 +2353,7 @@
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Moldova[z]</t>
+          <t>Moldova[aa]</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2373,7 +2373,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>[96]</t>
+          <t>[94]</t>
         </is>
       </c>
     </row>
@@ -2389,22 +2389,22 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>22585</t>
+          <t>23078</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>134</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>12937</t>
+          <t>13432</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>[97]</t>
+          <t>[95]</t>
         </is>
       </c>
     </row>
@@ -2415,7 +2415,7 @@
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Morocco[aa]</t>
+          <t>Morocco[ab]</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2435,7 +2435,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>[99]</t>
+          <t>[97]</t>
         </is>
       </c>
     </row>
@@ -2451,22 +2451,22 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>20850</t>
+          <t>20955</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>716</t>
+          <t>718</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>18528</t>
+          <t>18628</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>[100]</t>
+          <t>[98]</t>
         </is>
       </c>
     </row>
@@ -2477,27 +2477,27 @@
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Nepal</t>
+          <t>Kenya</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>19273</t>
+          <t>19913</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>325</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>14021</t>
+          <t>8121</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>[101][102]</t>
+          <t>[99]</t>
         </is>
       </c>
     </row>
@@ -2508,27 +2508,27 @@
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Kenya</t>
+          <t>Nepal</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>19125</t>
+          <t>19273</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>311</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>8021</t>
+          <t>14021</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>[103]</t>
+          <t>[100][101]</t>
         </is>
       </c>
     </row>
@@ -2559,7 +2559,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>[104][105]</t>
+          <t>[102][103]</t>
         </is>
       </c>
     </row>
@@ -2590,7 +2590,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>[106]</t>
+          <t>[104]</t>
         </is>
       </c>
     </row>
@@ -2621,7 +2621,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>[107]</t>
+          <t>[105]</t>
         </is>
       </c>
     </row>
@@ -2632,27 +2632,27 @@
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Czech Republic</t>
+          <t>Australia[ac]</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>16093</t>
+          <t>16303</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>374</t>
+          <t>189</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>11429</t>
+          <t>9758</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>[108]</t>
+          <t>[106]</t>
         </is>
       </c>
     </row>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>[109]</t>
+          <t>[107]</t>
         </is>
       </c>
     </row>
@@ -2694,27 +2694,27 @@
       <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Ivory Coast</t>
+          <t>Czech Republic</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>15813</t>
+          <t>16229</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>379</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>10793</t>
+          <t>11482</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>[110]</t>
+          <t>[108]</t>
         </is>
       </c>
     </row>
@@ -2725,27 +2725,27 @@
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Ethiopia</t>
+          <t>Ivory Coast</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>15810</t>
+          <t>15813</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>253</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>6685</t>
+          <t>10793</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>[111][112]</t>
+          <t>[109]</t>
         </is>
       </c>
     </row>
@@ -2756,27 +2756,27 @@
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Australia[ab]</t>
+          <t>Ethiopia</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>15582</t>
+          <t>15810</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>176</t>
+          <t>253</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>9619</t>
+          <t>6685</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>[113]</t>
+          <t>[110][111]</t>
         </is>
       </c>
     </row>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>[114]</t>
+          <t>[112]</t>
         </is>
       </c>
     </row>
@@ -2818,7 +2818,7 @@
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Denmark[ac]</t>
+          <t>Denmark[ad]</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>[115]</t>
+          <t>[113]</t>
         </is>
       </c>
     </row>
@@ -2849,27 +2849,27 @@
       <c r="B79" t="inlineStr"/>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Sudan</t>
+          <t>Palestine</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>11496</t>
+          <t>11548</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>725</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>6001</t>
+          <t>5015</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>[116]</t>
+          <t>[114]</t>
         </is>
       </c>
     </row>
@@ -2880,27 +2880,27 @@
       <c r="B80" t="inlineStr"/>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Palestine</t>
+          <t>Sudan</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>11284</t>
+          <t>11496</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>725</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>4833</t>
+          <t>6001</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>[117]</t>
+          <t>[115]</t>
         </is>
       </c>
     </row>
@@ -2916,22 +2916,22 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>11127</t>
+          <t>11444</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>328</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>5441</t>
+          <t>5586</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>[118]</t>
+          <t>[116]</t>
         </is>
       </c>
     </row>
@@ -2947,22 +2947,22 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>10871</t>
+          <t>11155</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>355</t>
+          <t>368</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>5766</t>
+          <t>5971</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>[119]</t>
+          <t>[117]</t>
         </is>
       </c>
     </row>
@@ -2973,27 +2973,27 @@
       <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr">
         <is>
-          <t>North Macedonia</t>
+          <t>Madagascar</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>10503</t>
+          <t>10748</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>476</t>
+          <t>105</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>5931</t>
+          <t>71461</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>[120][121]</t>
+          <t>[118]</t>
         </is>
       </c>
     </row>
@@ -3004,27 +3004,27 @@
       <c r="B84" t="inlineStr"/>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Madagascar</t>
+          <t>North Macedonia</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>10317</t>
+          <t>10617</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>480</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>7117</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>[122]</t>
+          <t>[119][120]</t>
         </is>
       </c>
     </row>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>9961</t>
+          <t>10106</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -3050,12 +3050,12 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>6655</t>
+          <t>6725</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>[123]</t>
+          <t>[121]</t>
         </is>
       </c>
     </row>
@@ -3066,12 +3066,12 @@
       <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Norway[ad]</t>
+          <t>Norway[ae]</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>9172</t>
+          <t>9185</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -3086,7 +3086,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>[126]</t>
+          <t>[124]</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>[127]</t>
+          <t>[125]</t>
         </is>
       </c>
     </row>
@@ -3128,7 +3128,7 @@
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr">
         <is>
-          <t>DR Congo[ae]</t>
+          <t>DR Congo[af]</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -3148,7 +3148,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>[128]</t>
+          <t>[126]</t>
         </is>
       </c>
     </row>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>[129]</t>
+          <t>[127]</t>
         </is>
       </c>
     </row>
@@ -3190,7 +3190,7 @@
       <c r="B90" t="inlineStr"/>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Finland[af]</t>
+          <t>Finland[ag]</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -3210,7 +3210,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>[132]</t>
+          <t>[130]</t>
         </is>
       </c>
     </row>
@@ -3241,7 +3241,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>[133]</t>
+          <t>[131]</t>
         </is>
       </c>
     </row>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>[134]</t>
+          <t>[132]</t>
         </is>
       </c>
     </row>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>7320</t>
+          <t>7366</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -3298,12 +3298,12 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>6103</t>
+          <t>6151</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>[135]</t>
+          <t>[133]</t>
         </is>
       </c>
     </row>
@@ -3334,7 +3334,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>[136][137]</t>
+          <t>[134][135]</t>
         </is>
       </c>
     </row>
@@ -3365,7 +3365,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>[138]</t>
+          <t>[136]</t>
         </is>
       </c>
     </row>
@@ -3396,7 +3396,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>[139]</t>
+          <t>[137]</t>
         </is>
       </c>
     </row>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>[140][141]</t>
+          <t>[138][139]</t>
         </is>
       </c>
     </row>
@@ -3458,7 +3458,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>[142][143]</t>
+          <t>[140][141]</t>
         </is>
       </c>
     </row>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>[144]</t>
+          <t>[142]</t>
         </is>
       </c>
     </row>
@@ -3520,7 +3520,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>[145]</t>
+          <t>[143]</t>
         </is>
       </c>
     </row>
@@ -3551,7 +3551,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>[146]</t>
+          <t>[144]</t>
         </is>
       </c>
     </row>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>[147]</t>
+          <t>[145]</t>
         </is>
       </c>
     </row>
@@ -3613,7 +3613,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>[148]</t>
+          <t>[146]</t>
         </is>
       </c>
     </row>
@@ -3644,7 +3644,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>[149]</t>
+          <t>[147]</t>
         </is>
       </c>
     </row>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>[150]</t>
+          <t>[148]</t>
         </is>
       </c>
     </row>
@@ -3706,7 +3706,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>[151]</t>
+          <t>[149]</t>
         </is>
       </c>
     </row>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>[152]</t>
+          <t>[150]</t>
         </is>
       </c>
     </row>
@@ -3768,7 +3768,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>[78][153]</t>
+          <t>[76][151]</t>
         </is>
       </c>
     </row>
@@ -3799,7 +3799,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>[154]</t>
+          <t>[152]</t>
         </is>
       </c>
     </row>
@@ -3830,7 +3830,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>[155]</t>
+          <t>[153]</t>
         </is>
       </c>
     </row>
@@ -3861,7 +3861,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>[156][157]</t>
+          <t>[154][155]</t>
         </is>
       </c>
     </row>
@@ -3872,7 +3872,7 @@
       <c r="B112" t="inlineStr"/>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Somalia[ag]</t>
+          <t>Somalia[ah]</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3892,7 +3892,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>[158]</t>
+          <t>[156]</t>
         </is>
       </c>
     </row>
@@ -3903,7 +3903,7 @@
       <c r="B113" t="inlineStr"/>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Congo[ah]</t>
+          <t>Congo[ai]</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3923,7 +3923,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>[159][160]</t>
+          <t>[157][158]</t>
         </is>
       </c>
     </row>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>[161]</t>
+          <t>[159]</t>
         </is>
       </c>
     </row>
@@ -3985,7 +3985,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>[162]</t>
+          <t>[160]</t>
         </is>
       </c>
     </row>
@@ -4016,7 +4016,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>[163]</t>
+          <t>[161]</t>
         </is>
       </c>
     </row>
@@ -4047,7 +4047,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>[164][165]</t>
+          <t>[162][163]</t>
         </is>
       </c>
     </row>
@@ -4078,7 +4078,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>[166]</t>
+          <t>[164]</t>
         </is>
       </c>
     </row>
@@ -4089,7 +4089,7 @@
       <c r="B119" t="inlineStr"/>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Cuba[ai]</t>
+          <t>Cuba[aj]</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>[167]</t>
+          <t>[165]</t>
         </is>
       </c>
     </row>
@@ -4140,7 +4140,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>[168]</t>
+          <t>[166]</t>
         </is>
       </c>
     </row>
@@ -4171,7 +4171,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>[169]</t>
+          <t>[167]</t>
         </is>
       </c>
     </row>
@@ -4202,7 +4202,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>[170]</t>
+          <t>[168]</t>
         </is>
       </c>
     </row>
@@ -4233,7 +4233,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>[171][172]</t>
+          <t>[169][170]</t>
         </is>
       </c>
     </row>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>[173]</t>
+          <t>[171]</t>
         </is>
       </c>
     </row>
@@ -4295,7 +4295,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>[174][175]</t>
+          <t>[172][173]</t>
         </is>
       </c>
     </row>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>[176]</t>
+          <t>[174]</t>
         </is>
       </c>
     </row>
@@ -4337,27 +4337,27 @@
       <c r="B127" t="inlineStr"/>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Estonia</t>
+          <t>Namibia</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>2042</t>
+          <t>2052</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>1926</t>
+          <t>164</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>[177]</t>
+          <t>[175][176]</t>
         </is>
       </c>
     </row>
@@ -4368,27 +4368,27 @@
       <c r="B128" t="inlineStr"/>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Namibia</t>
+          <t>Estonia</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>1986</t>
+          <t>2042</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>69</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>1926</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>[178][179]</t>
+          <t>[177]</t>
         </is>
       </c>
     </row>
@@ -4419,7 +4419,7 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>[180][181]</t>
+          <t>[178][179]</t>
         </is>
       </c>
     </row>
@@ -4450,7 +4450,7 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>[182]</t>
+          <t>[180]</t>
         </is>
       </c>
     </row>
@@ -4481,7 +4481,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>[183]</t>
+          <t>[181]</t>
         </is>
       </c>
     </row>
@@ -4497,7 +4497,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>1803</t>
+          <t>1818</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -4507,12 +4507,12 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>1355</t>
+          <t>1362</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>[184][185]</t>
+          <t>[182][183]</t>
         </is>
       </c>
     </row>
@@ -4523,27 +4523,27 @@
       <c r="B133" t="inlineStr"/>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Benin</t>
+          <t>Mozambique</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>1770</t>
+          <t>1808</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>11</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>1036</t>
+          <t>638</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>[186]</t>
+          <t>[184]</t>
         </is>
       </c>
     </row>
@@ -4554,27 +4554,27 @@
       <c r="B134" t="inlineStr"/>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Mozambique</t>
+          <t>Benin</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>1748</t>
+          <t>1770</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>616</t>
+          <t>1036</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>[187]</t>
+          <t>[185]</t>
         </is>
       </c>
     </row>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>[188]</t>
+          <t>[186]</t>
         </is>
       </c>
     </row>
@@ -4616,7 +4616,7 @@
       <c r="B136" t="inlineStr"/>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Donetsk PR[aj]</t>
+          <t>Donetsk PR[ak]</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4636,7 +4636,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>[189]</t>
+          <t>[187]</t>
         </is>
       </c>
     </row>
@@ -4667,7 +4667,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>[190]</t>
+          <t>[188]</t>
         </is>
       </c>
     </row>
@@ -4698,7 +4698,7 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>[191]</t>
+          <t>[189]</t>
         </is>
       </c>
     </row>
@@ -4729,7 +4729,7 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>[78][192]</t>
+          <t>[76][190]</t>
         </is>
       </c>
     </row>
@@ -4740,7 +4740,7 @@
       <c r="B140" t="inlineStr"/>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Uruguay[ak]</t>
+          <t>Uruguay[al]</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4760,7 +4760,7 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>[193]</t>
+          <t>[191]</t>
         </is>
       </c>
     </row>
@@ -4791,7 +4791,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>[194]</t>
+          <t>[192]</t>
         </is>
       </c>
     </row>
@@ -4822,7 +4822,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>[195]</t>
+          <t>[193]</t>
         </is>
       </c>
     </row>
@@ -4853,7 +4853,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>[196]</t>
+          <t>[194]</t>
         </is>
       </c>
     </row>
@@ -4864,7 +4864,7 @@
       <c r="B144" t="inlineStr"/>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Georgia[al]</t>
+          <t>Georgia[am]</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4884,7 +4884,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>[197]</t>
+          <t>[195]</t>
         </is>
       </c>
     </row>
@@ -4915,7 +4915,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>[198][199]</t>
+          <t>[196][197]</t>
         </is>
       </c>
     </row>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>[200]</t>
+          <t>[198]</t>
         </is>
       </c>
     </row>
@@ -4977,7 +4977,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>[201][202]</t>
+          <t>[199][200]</t>
         </is>
       </c>
     </row>
@@ -4988,7 +4988,7 @@
       <c r="B148" t="inlineStr"/>
       <c r="C148" t="inlineStr">
         <is>
-          <t>USS Theodore Roosevelt[am]</t>
+          <t>USS Theodore Roosevelt[an]</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -5008,7 +5008,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>[203][204]</t>
+          <t>[201][202]</t>
         </is>
       </c>
     </row>
@@ -5019,7 +5019,7 @@
       <c r="B149" t="inlineStr"/>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Charles de Gaulle[an]</t>
+          <t>Charles de Gaulle[ao]</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -5039,7 +5039,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>[205]</t>
+          <t>[203]</t>
         </is>
       </c>
     </row>
@@ -5050,7 +5050,7 @@
       <c r="B150" t="inlineStr"/>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Cyprus[ao]</t>
+          <t>Cyprus[ap]</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -5070,7 +5070,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>[209]</t>
+          <t>[207]</t>
         </is>
       </c>
     </row>
@@ -5101,7 +5101,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>[210]</t>
+          <t>[208]</t>
         </is>
       </c>
     </row>
@@ -5132,7 +5132,7 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>[211]</t>
+          <t>[209]</t>
         </is>
       </c>
     </row>
@@ -5148,7 +5148,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>918</t>
+          <t>922</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -5158,12 +5158,12 @@
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>804</t>
+          <t>806</t>
         </is>
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>[212]</t>
+          <t>[210]</t>
         </is>
       </c>
     </row>
@@ -5194,7 +5194,7 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>[213]</t>
+          <t>[211]</t>
         </is>
       </c>
     </row>
@@ -5225,7 +5225,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>[214]</t>
+          <t>[212]</t>
         </is>
       </c>
     </row>
@@ -5256,7 +5256,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>[215][216]</t>
+          <t>[213][214]</t>
         </is>
       </c>
     </row>
@@ -5267,27 +5267,27 @@
       <c r="B157" t="inlineStr"/>
       <c r="C157" t="inlineStr">
         <is>
-          <t>Botswana[ap]</t>
+          <t>Malta</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>804</t>
+          <t>814</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>665</t>
         </is>
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>[218]</t>
+          <t>[215]</t>
         </is>
       </c>
     </row>
@@ -5298,27 +5298,27 @@
       <c r="B158" t="inlineStr"/>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Malta</t>
+          <t>Botswana[aq]</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>720</t>
+          <t>804</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>665</t>
+          <t>63</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>[219]</t>
+          <t>[217]</t>
         </is>
       </c>
     </row>
@@ -5329,7 +5329,7 @@
       <c r="B159" t="inlineStr"/>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Syria[aq]</t>
+          <t>Syria[ar]</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -5349,7 +5349,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>[220]</t>
+          <t>[218]</t>
         </is>
       </c>
     </row>
@@ -5380,7 +5380,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>[221][222]</t>
+          <t>[219][220]</t>
         </is>
       </c>
     </row>
@@ -5411,7 +5411,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>[223]</t>
+          <t>[221]</t>
         </is>
       </c>
     </row>
@@ -5422,7 +5422,7 @@
       <c r="B162" t="inlineStr"/>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Luhansk PR[aj]</t>
+          <t>Luhansk PR[ak]</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -5442,7 +5442,7 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>[224]</t>
+          <t>[222]</t>
         </is>
       </c>
     </row>
@@ -5473,7 +5473,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>[225]</t>
+          <t>[223]</t>
         </is>
       </c>
     </row>
@@ -5484,7 +5484,7 @@
       <c r="B164" t="inlineStr"/>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Somaliland[ar]</t>
+          <t>Somaliland[as]</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -5504,7 +5504,7 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>[226]</t>
+          <t>[224]</t>
         </is>
       </c>
     </row>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>[227]</t>
+          <t>[225]</t>
         </is>
       </c>
     </row>
@@ -5546,7 +5546,7 @@
       <c r="B166" t="inlineStr"/>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Taiwan[as]</t>
+          <t>Taiwan[at]</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -5566,7 +5566,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>[229]</t>
+          <t>[227]</t>
         </is>
       </c>
     </row>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>[230]</t>
+          <t>[228]</t>
         </is>
       </c>
     </row>
@@ -5628,7 +5628,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>[231]</t>
+          <t>[229]</t>
         </is>
       </c>
     </row>
@@ -5659,7 +5659,7 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>[232]</t>
+          <t>[230]</t>
         </is>
       </c>
     </row>
@@ -5690,7 +5690,7 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>[233]</t>
+          <t>[231]</t>
         </is>
       </c>
     </row>
@@ -5721,7 +5721,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>[234]</t>
+          <t>[232]</t>
         </is>
       </c>
     </row>
@@ -5752,7 +5752,7 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>[235]</t>
+          <t>[233]</t>
         </is>
       </c>
     </row>
@@ -5763,7 +5763,7 @@
       <c r="B173" t="inlineStr"/>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Guam[am]</t>
+          <t>Guam[an]</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -5783,7 +5783,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>[9][236]</t>
+          <t>[9][234]</t>
         </is>
       </c>
     </row>
@@ -5814,7 +5814,7 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>[237]</t>
+          <t>[235]</t>
         </is>
       </c>
     </row>
@@ -5825,7 +5825,7 @@
       <c r="B175" t="inlineStr"/>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Isle of Man[at]</t>
+          <t>Isle of Man[au]</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -5845,7 +5845,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>[238]</t>
+          <t>[236]</t>
         </is>
       </c>
     </row>
@@ -5876,7 +5876,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>[239]</t>
+          <t>[237]</t>
         </is>
       </c>
     </row>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>[240]</t>
+          <t>[238]</t>
         </is>
       </c>
     </row>
@@ -5938,7 +5938,7 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>[241]</t>
+          <t>[239]</t>
         </is>
       </c>
     </row>
@@ -5969,7 +5969,7 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>[242]</t>
+          <t>[240]</t>
         </is>
       </c>
     </row>
@@ -6000,7 +6000,7 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>[243]</t>
+          <t>[241]</t>
         </is>
       </c>
     </row>
@@ -6031,7 +6031,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>[244][245]</t>
+          <t>[242][243]</t>
         </is>
       </c>
     </row>
@@ -6062,7 +6062,7 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>[246]</t>
+          <t>[244]</t>
         </is>
       </c>
     </row>
@@ -6073,7 +6073,7 @@
       <c r="B183" t="inlineStr"/>
       <c r="C183" t="inlineStr">
         <is>
-          <t>Artsakh[au]</t>
+          <t>Artsakh[av]</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
@@ -6093,7 +6093,7 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>[247]</t>
+          <t>[245]</t>
         </is>
       </c>
     </row>
@@ -6124,7 +6124,7 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>[248]</t>
+          <t>[246]</t>
         </is>
       </c>
     </row>
@@ -6155,7 +6155,7 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>[249]</t>
+          <t>[247]</t>
         </is>
       </c>
     </row>
@@ -6186,7 +6186,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>[250]</t>
+          <t>[248]</t>
         </is>
       </c>
     </row>
@@ -6217,7 +6217,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>[251]</t>
+          <t>[249]</t>
         </is>
       </c>
     </row>
@@ -6248,7 +6248,7 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>[252][253]</t>
+          <t>[250][251]</t>
         </is>
       </c>
     </row>
@@ -6279,7 +6279,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>[254][255]</t>
+          <t>[252][253]</t>
         </is>
       </c>
     </row>
@@ -6290,7 +6290,7 @@
       <c r="B190" t="inlineStr"/>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Northern Cyprus[av]</t>
+          <t>Northern Cyprus[aw]</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -6310,7 +6310,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>[256]</t>
+          <t>[254]</t>
         </is>
       </c>
     </row>
@@ -6321,7 +6321,7 @@
       <c r="B191" t="inlineStr"/>
       <c r="C191" t="inlineStr">
         <is>
-          <t>Greg Mortimer[ak]</t>
+          <t>Greg Mortimer[al]</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -6341,7 +6341,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>[257][258]</t>
+          <t>[255][256]</t>
         </is>
       </c>
     </row>
@@ -6372,7 +6372,7 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>[259]</t>
+          <t>[257]</t>
         </is>
       </c>
     </row>
@@ -6388,7 +6388,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>119</t>
+          <t>120</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
@@ -6398,12 +6398,12 @@
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>105</t>
         </is>
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>[260]</t>
+          <t>[258]</t>
         </is>
       </c>
     </row>
@@ -6434,7 +6434,7 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>[261]</t>
+          <t>[259]</t>
         </is>
       </c>
     </row>
@@ -6465,7 +6465,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>[262]</t>
+          <t>[260]</t>
         </is>
       </c>
     </row>
@@ -6496,7 +6496,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>[263]</t>
+          <t>[261]</t>
         </is>
       </c>
     </row>
@@ -6527,7 +6527,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>[264]</t>
+          <t>[262]</t>
         </is>
       </c>
     </row>
@@ -6558,7 +6558,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>[265]</t>
+          <t>[263]</t>
         </is>
       </c>
     </row>
@@ -6589,7 +6589,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>[266]</t>
+          <t>[264]</t>
         </is>
       </c>
     </row>
@@ -6600,7 +6600,7 @@
       <c r="B200" t="inlineStr"/>
       <c r="C200" t="inlineStr">
         <is>
-          <t>South Ossetia[aw]</t>
+          <t>South Ossetia[ax]</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
@@ -6620,7 +6620,7 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>[247]</t>
+          <t>[245]</t>
         </is>
       </c>
     </row>
@@ -6651,7 +6651,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>[267][268]</t>
+          <t>[265][266]</t>
         </is>
       </c>
     </row>
@@ -6682,7 +6682,7 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>[269]</t>
+          <t>[267]</t>
         </is>
       </c>
     </row>
@@ -6713,7 +6713,7 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>[270]</t>
+          <t>[268]</t>
         </is>
       </c>
     </row>
@@ -6724,7 +6724,7 @@
       <c r="B204" t="inlineStr"/>
       <c r="C204" t="inlineStr">
         <is>
-          <t>Abkhazia[ax]</t>
+          <t>Abkhazia[ay]</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
@@ -6744,7 +6744,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>[247]</t>
+          <t>[245]</t>
         </is>
       </c>
     </row>
@@ -6755,7 +6755,7 @@
       <c r="B205" t="inlineStr"/>
       <c r="C205" t="inlineStr">
         <is>
-          <t>Saint Vincent[ay]</t>
+          <t>Saint Vincent[az]</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
@@ -6775,7 +6775,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>[271]</t>
+          <t>[269]</t>
         </is>
       </c>
     </row>
@@ -6806,7 +6806,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>[272]</t>
+          <t>[270]</t>
         </is>
       </c>
     </row>
@@ -6837,7 +6837,7 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>[273]</t>
+          <t>[271]</t>
         </is>
       </c>
     </row>
@@ -6868,7 +6868,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>[274]</t>
+          <t>[272]</t>
         </is>
       </c>
     </row>
@@ -6899,7 +6899,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>[275]</t>
+          <t>[273]</t>
         </is>
       </c>
     </row>
@@ -6930,7 +6930,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>[276]</t>
+          <t>[274]</t>
         </is>
       </c>
     </row>
@@ -6961,7 +6961,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>[277][278]</t>
+          <t>[275][276]</t>
         </is>
       </c>
     </row>
@@ -6992,7 +6992,7 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>[279][280]</t>
+          <t>[277][278]</t>
         </is>
       </c>
     </row>
@@ -7023,7 +7023,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>[281]</t>
+          <t>[279]</t>
         </is>
       </c>
     </row>
@@ -7054,7 +7054,7 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>[282]</t>
+          <t>[280]</t>
         </is>
       </c>
     </row>
@@ -7085,7 +7085,7 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>[283]</t>
+          <t>[281]</t>
         </is>
       </c>
     </row>
@@ -7116,7 +7116,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>[284]</t>
+          <t>[282]</t>
         </is>
       </c>
     </row>
@@ -7147,7 +7147,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>[285]</t>
+          <t>[283]</t>
         </is>
       </c>
     </row>
@@ -7178,7 +7178,7 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>[286]</t>
+          <t>[284]</t>
         </is>
       </c>
     </row>
@@ -7209,7 +7209,7 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>[287]</t>
+          <t>[285]</t>
         </is>
       </c>
     </row>
@@ -7220,7 +7220,7 @@
       <c r="B220" t="inlineStr"/>
       <c r="C220" t="inlineStr">
         <is>
-          <t>MS Zaandam[az]</t>
+          <t>MS Zaandam[ba]</t>
         </is>
       </c>
       <c r="D220" t="inlineStr">
@@ -7240,7 +7240,7 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>[290][291]</t>
+          <t>[288][289]</t>
         </is>
       </c>
     </row>
@@ -7251,7 +7251,7 @@
       <c r="B221" t="inlineStr"/>
       <c r="C221" t="inlineStr">
         <is>
-          <t>Coral Princess[ba]</t>
+          <t>Coral Princess[bb]</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
@@ -7271,7 +7271,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>[293]</t>
+          <t>[291]</t>
         </is>
       </c>
     </row>
@@ -7302,7 +7302,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>[294]</t>
+          <t>[292]</t>
         </is>
       </c>
     </row>
@@ -7333,7 +7333,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>[295]</t>
+          <t>[293]</t>
         </is>
       </c>
     </row>
@@ -7364,7 +7364,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>[296]</t>
+          <t>[294]</t>
         </is>
       </c>
     </row>
@@ -7375,7 +7375,7 @@
       <c r="B225" t="inlineStr"/>
       <c r="C225" t="inlineStr">
         <is>
-          <t>HNLMS Dolfijn[bb]</t>
+          <t>HNLMS Dolfijn[bc]</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
@@ -7395,7 +7395,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>[297][300]</t>
+          <t>[295][298]</t>
         </is>
       </c>
     </row>
@@ -7426,7 +7426,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>[301]</t>
+          <t>[299]</t>
         </is>
       </c>
     </row>
@@ -7457,7 +7457,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>[302]</t>
+          <t>[300]</t>
         </is>
       </c>
     </row>
@@ -7488,7 +7488,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>[303]</t>
+          <t>[301]</t>
         </is>
       </c>
     </row>
@@ -7519,7 +7519,7 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>[304]</t>
+          <t>[302]</t>
         </is>
       </c>
     </row>
@@ -7550,7 +7550,7 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>[305]</t>
+          <t>[303]</t>
         </is>
       </c>
     </row>
@@ -7561,7 +7561,7 @@
       <c r="B231" t="inlineStr"/>
       <c r="C231" t="inlineStr">
         <is>
-          <t>Tanzania[bc]</t>
+          <t>Tanzania[bd]</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
@@ -7581,7 +7581,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>[307][308]</t>
+          <t>[305][306]</t>
         </is>
       </c>
     </row>
@@ -7626,32 +7626,32 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reporte]d to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations.The total number of cases may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Deaths: Reporting criteria vary between locations.The total number of deaths may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations.The total number of recoveries may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ WorldTotal numbers worldwide. Some locations, including North Korea, have yet to report cases. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[10][11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as a "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[22]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[23] In the latest report (11 July 2020), the number of total deaths is 11,227.[24] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[27] ^ SpainExcludes serology–confirmed cases. ^ GermanyNot all state authorities count recoveries.[38]Recoveries include estimations by the Robert Koch Institute.[38][39] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[40]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[40] ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[41] ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[45] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[46] ^ EgyptIncludes cases identified on the MS River Anuket. ^ ChinaExcluding 280 asymptomatic cases under medical observation as of 29 July 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[64] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[71] ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ MoldovaIncluding the disputed territory of Transnistria. ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[98] ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[124] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[125] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[130] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[131] ^ SomaliaExcluding the de facto state of Somaliland. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[205] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[206][207][208] ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana243 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[217] ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomalilandCases from this de facto state are not counted by Somalia. ^ TaiwanIncluding cases from the ROCS Pan Shi.[228] ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[238] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[288][289]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[292]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[297]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[298][299] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[306] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[307][308]</t>
+          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reporte]d to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations.The total number of cases may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Deaths: Reporting criteria vary between locations.The total number of deaths may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations.The total number of recoveries may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ WorldTotal numbers worldwide. Some locations, including North Korea, have yet to report cases. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[10][11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as a "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[22]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[23] In the latest report (11 July 2020), the number of total deaths is 11,227.[24] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[26] ^ SpainExcludes serology–confirmed cases. ^ GermanyNot all state authorities count recoveries.[37]Recoveries include estimations by the Robert Koch Institute.[37][38] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[39]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[39] ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[40] ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[44] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[45] ^ EgyptIncludes cases identified on the MS River Anuket. ^ ChinaExcluding 280 asymptomatic cases under medical observation as of 29 July 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[62] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[69] ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ IrelandExcluding confirmed cases and deaths in Northern Ireland. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ MoldovaIncluding the disputed territory of Transnistria. ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[96] ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[122] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[123] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[128] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[129] ^ SomaliaExcluding the de facto state of Somaliland. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[203] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[204][205][206] ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana243 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[216] ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomalilandCases from this de facto state are not counted by Somalia. ^ TaiwanIncluding cases from the ROCS Pan Shi.[226] ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[236] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[286][287]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[290]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[295]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[296][297] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[304] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[305][306]</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reporte]d to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations.The total number of cases may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Deaths: Reporting criteria vary between locations.The total number of deaths may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations.The total number of recoveries may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ WorldTotal numbers worldwide. Some locations, including North Korea, have yet to report cases. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[10][11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as a "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[22]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[23] In the latest report (11 July 2020), the number of total deaths is 11,227.[24] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[27] ^ SpainExcludes serology–confirmed cases. ^ GermanyNot all state authorities count recoveries.[38]Recoveries include estimations by the Robert Koch Institute.[38][39] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[40]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[40] ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[41] ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[45] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[46] ^ EgyptIncludes cases identified on the MS River Anuket. ^ ChinaExcluding 280 asymptomatic cases under medical observation as of 29 July 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[64] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[71] ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ MoldovaIncluding the disputed territory of Transnistria. ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[98] ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[124] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[125] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[130] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[131] ^ SomaliaExcluding the de facto state of Somaliland. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[205] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[206][207][208] ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana243 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[217] ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomalilandCases from this de facto state are not counted by Somalia. ^ TaiwanIncluding cases from the ROCS Pan Shi.[228] ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[238] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[288][289]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[292]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[297]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[298][299] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[306] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[307][308]</t>
+          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reporte]d to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations.The total number of cases may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Deaths: Reporting criteria vary between locations.The total number of deaths may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations.The total number of recoveries may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ WorldTotal numbers worldwide. Some locations, including North Korea, have yet to report cases. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[10][11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as a "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[22]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[23] In the latest report (11 July 2020), the number of total deaths is 11,227.[24] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[26] ^ SpainExcludes serology–confirmed cases. ^ GermanyNot all state authorities count recoveries.[37]Recoveries include estimations by the Robert Koch Institute.[37][38] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[39]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[39] ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[40] ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[44] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[45] ^ EgyptIncludes cases identified on the MS River Anuket. ^ ChinaExcluding 280 asymptomatic cases under medical observation as of 29 July 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[62] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[69] ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ IrelandExcluding confirmed cases and deaths in Northern Ireland. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ MoldovaIncluding the disputed territory of Transnistria. ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[96] ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[122] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[123] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[128] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[129] ^ SomaliaExcluding the de facto state of Somaliland. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[203] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[204][205][206] ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana243 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[216] ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomalilandCases from this de facto state are not counted by Somalia. ^ TaiwanIncluding cases from the ROCS Pan Shi.[226] ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[236] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[286][287]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[290]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[295]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[296][297] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[304] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[305][306]</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reporte]d to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations.The total number of cases may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Deaths: Reporting criteria vary between locations.The total number of deaths may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations.The total number of recoveries may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ WorldTotal numbers worldwide. Some locations, including North Korea, have yet to report cases. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[10][11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as a "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[22]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[23] In the latest report (11 July 2020), the number of total deaths is 11,227.[24] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[27] ^ SpainExcludes serology–confirmed cases. ^ GermanyNot all state authorities count recoveries.[38]Recoveries include estimations by the Robert Koch Institute.[38][39] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[40]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[40] ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[41] ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[45] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[46] ^ EgyptIncludes cases identified on the MS River Anuket. ^ ChinaExcluding 280 asymptomatic cases under medical observation as of 29 July 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[64] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[71] ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ MoldovaIncluding the disputed territory of Transnistria. ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[98] ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[124] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[125] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[130] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[131] ^ SomaliaExcluding the de facto state of Somaliland. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[205] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[206][207][208] ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana243 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[217] ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomalilandCases from this de facto state are not counted by Somalia. ^ TaiwanIncluding cases from the ROCS Pan Shi.[228] ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[238] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[288][289]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[292]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[297]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[298][299] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[306] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[307][308]</t>
+          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reporte]d to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations.The total number of cases may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Deaths: Reporting criteria vary between locations.The total number of deaths may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations.The total number of recoveries may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ WorldTotal numbers worldwide. Some locations, including North Korea, have yet to report cases. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[10][11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as a "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[22]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[23] In the latest report (11 July 2020), the number of total deaths is 11,227.[24] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[26] ^ SpainExcludes serology–confirmed cases. ^ GermanyNot all state authorities count recoveries.[37]Recoveries include estimations by the Robert Koch Institute.[37][38] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[39]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[39] ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[40] ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[44] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[45] ^ EgyptIncludes cases identified on the MS River Anuket. ^ ChinaExcluding 280 asymptomatic cases under medical observation as of 29 July 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[62] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[69] ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ IrelandExcluding confirmed cases and deaths in Northern Ireland. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ MoldovaIncluding the disputed territory of Transnistria. ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[96] ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[122] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[123] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[128] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[129] ^ SomaliaExcluding the de facto state of Somaliland. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[203] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[204][205][206] ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana243 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[216] ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomalilandCases from this de facto state are not counted by Somalia. ^ TaiwanIncluding cases from the ROCS Pan Shi.[226] ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[236] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[286][287]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[290]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[295]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[296][297] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[304] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[305][306]</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reporte]d to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations.The total number of cases may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Deaths: Reporting criteria vary between locations.The total number of deaths may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations.The total number of recoveries may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ WorldTotal numbers worldwide. Some locations, including North Korea, have yet to report cases. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[10][11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as a "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[22]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[23] In the latest report (11 July 2020), the number of total deaths is 11,227.[24] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[27] ^ SpainExcludes serology–confirmed cases. ^ GermanyNot all state authorities count recoveries.[38]Recoveries include estimations by the Robert Koch Institute.[38][39] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[40]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[40] ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[41] ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[45] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[46] ^ EgyptIncludes cases identified on the MS River Anuket. ^ ChinaExcluding 280 asymptomatic cases under medical observation as of 29 July 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[64] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[71] ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ MoldovaIncluding the disputed territory of Transnistria. ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[98] ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[124] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[125] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[130] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[131] ^ SomaliaExcluding the de facto state of Somaliland. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[205] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[206][207][208] ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana243 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[217] ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomalilandCases from this de facto state are not counted by Somalia. ^ TaiwanIncluding cases from the ROCS Pan Shi.[228] ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[238] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[288][289]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[292]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[297]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[298][299] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[306] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[307][308]</t>
+          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reporte]d to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations.The total number of cases may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Deaths: Reporting criteria vary between locations.The total number of deaths may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations.The total number of recoveries may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ WorldTotal numbers worldwide. Some locations, including North Korea, have yet to report cases. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[10][11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as a "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[22]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[23] In the latest report (11 July 2020), the number of total deaths is 11,227.[24] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[26] ^ SpainExcludes serology–confirmed cases. ^ GermanyNot all state authorities count recoveries.[37]Recoveries include estimations by the Robert Koch Institute.[37][38] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[39]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[39] ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[40] ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[44] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[45] ^ EgyptIncludes cases identified on the MS River Anuket. ^ ChinaExcluding 280 asymptomatic cases under medical observation as of 29 July 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[62] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[69] ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ IrelandExcluding confirmed cases and deaths in Northern Ireland. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ MoldovaIncluding the disputed territory of Transnistria. ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[96] ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[122] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[123] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[128] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[129] ^ SomaliaExcluding the de facto state of Somaliland. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[203] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[204][205][206] ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana243 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[216] ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomalilandCases from this de facto state are not counted by Somalia. ^ TaiwanIncluding cases from the ROCS Pan Shi.[226] ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[236] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[286][287]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[290]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[295]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[296][297] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[304] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[305][306]</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
         <is>
-          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reporte]d to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations.The total number of cases may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Deaths: Reporting criteria vary between locations.The total number of deaths may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations.The total number of recoveries may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ WorldTotal numbers worldwide. Some locations, including North Korea, have yet to report cases. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[10][11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as a "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[22]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[23] In the latest report (11 July 2020), the number of total deaths is 11,227.[24] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[27] ^ SpainExcludes serology–confirmed cases. ^ GermanyNot all state authorities count recoveries.[38]Recoveries include estimations by the Robert Koch Institute.[38][39] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[40]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[40] ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[41] ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[45] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[46] ^ EgyptIncludes cases identified on the MS River Anuket. ^ ChinaExcluding 280 asymptomatic cases under medical observation as of 29 July 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[64] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[71] ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ MoldovaIncluding the disputed territory of Transnistria. ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[98] ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[124] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[125] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[130] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[131] ^ SomaliaExcluding the de facto state of Somaliland. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[205] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[206][207][208] ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana243 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[217] ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomalilandCases from this de facto state are not counted by Somalia. ^ TaiwanIncluding cases from the ROCS Pan Shi.[228] ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[238] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[288][289]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[292]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[297]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[298][299] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[306] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[307][308]</t>
+          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reporte]d to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations.The total number of cases may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Deaths: Reporting criteria vary between locations.The total number of deaths may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations.The total number of recoveries may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ WorldTotal numbers worldwide. Some locations, including North Korea, have yet to report cases. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[10][11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as a "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[22]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[23] In the latest report (11 July 2020), the number of total deaths is 11,227.[24] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[26] ^ SpainExcludes serology–confirmed cases. ^ GermanyNot all state authorities count recoveries.[37]Recoveries include estimations by the Robert Koch Institute.[37][38] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[39]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[39] ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[40] ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[44] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[45] ^ EgyptIncludes cases identified on the MS River Anuket. ^ ChinaExcluding 280 asymptomatic cases under medical observation as of 29 July 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[62] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[69] ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ IrelandExcluding confirmed cases and deaths in Northern Ireland. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ MoldovaIncluding the disputed territory of Transnistria. ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[96] ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[122] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[123] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[128] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[129] ^ SomaliaExcluding the de facto state of Somaliland. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[203] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[204][205][206] ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana243 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[216] ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomalilandCases from this de facto state are not counted by Somalia. ^ TaiwanIncluding cases from the ROCS Pan Shi.[226] ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[236] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[286][287]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[290]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[295]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[296][297] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[304] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[305][306]</t>
         </is>
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reporte]d to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations.The total number of cases may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Deaths: Reporting criteria vary between locations.The total number of deaths may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations.The total number of recoveries may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ WorldTotal numbers worldwide. Some locations, including North Korea, have yet to report cases. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[10][11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as a "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[22]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[23] In the latest report (11 July 2020), the number of total deaths is 11,227.[24] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[27] ^ SpainExcludes serology–confirmed cases. ^ GermanyNot all state authorities count recoveries.[38]Recoveries include estimations by the Robert Koch Institute.[38][39] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[40]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[40] ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[41] ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[45] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[46] ^ EgyptIncludes cases identified on the MS River Anuket. ^ ChinaExcluding 280 asymptomatic cases under medical observation as of 29 July 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[64] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[71] ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ MoldovaIncluding the disputed territory of Transnistria. ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[98] ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[124] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[125] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[130] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[131] ^ SomaliaExcluding the de facto state of Somaliland. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[205] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[206][207][208] ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana243 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[217] ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomalilandCases from this de facto state are not counted by Somalia. ^ TaiwanIncluding cases from the ROCS Pan Shi.[228] ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[238] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[288][289]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[292]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[297]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[298][299] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[306] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[307][308]</t>
+          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reporte]d to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations.The total number of cases may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Deaths: Reporting criteria vary between locations.The total number of deaths may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations.The total number of recoveries may not necessarily represent an aggregate sum of all entries in this column as it relies on aggregate sources and not local sources. ^ WorldTotal numbers worldwide. Some locations, including North Korea, have yet to report cases. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[10][11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as a "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[22]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[23] In the latest report (11 July 2020), the number of total deaths is 11,227.[24] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[26] ^ SpainExcludes serology–confirmed cases. ^ GermanyNot all state authorities count recoveries.[37]Recoveries include estimations by the Robert Koch Institute.[37][38] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[39]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[39] ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[40] ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[44] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[45] ^ EgyptIncludes cases identified on the MS River Anuket. ^ ChinaExcluding 280 asymptomatic cases under medical observation as of 29 July 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[62] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[69] ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ IrelandExcluding confirmed cases and deaths in Northern Ireland. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ MoldovaIncluding the disputed territory of Transnistria. ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[96] ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[122] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[123] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[128] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[129] ^ SomaliaExcluding the de facto state of Somaliland. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[203] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[204][205][206] ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana243 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[216] ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomalilandCases from this de facto state are not counted by Somalia. ^ TaiwanIncluding cases from the ROCS Pan Shi.[226] ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[236] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[286][287]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[290]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[295]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[296][297] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[304] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[305][306]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update covid sample data
</commit_message>
<xml_diff>
--- a/class1_explore/scrapers/covid_wiki_stats.xlsx
+++ b/class1_explore/scrapers/covid_wiki_stats.xlsx
@@ -498,17 +498,17 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>30,290,791</t>
+          <t>30,566,740</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>947,919</t>
+          <t>953,072</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>20,623,028</t>
+          <t>20,827,524</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -529,17 +529,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>6780553</t>
+          <t>6819709</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>200985</t>
+          <t>201735</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>3659384</t>
+          <t>3689081</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -560,17 +560,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>5214677</t>
+          <t>5308014</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>84372</t>
+          <t>85619</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>4112551</t>
+          <t>4208431</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -591,17 +591,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4455386</t>
+          <t>4497434</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>134935</t>
+          <t>135857</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>3753082</t>
+          <t>3789139</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -622,17 +622,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1091186</t>
+          <t>1097251</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>19195</t>
+          <t>19339</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>901207</t>
+          <t>906462</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -653,17 +653,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>750098</t>
+          <t>756412</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>31146</t>
+          <t>31283</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>594513</t>
+          <t>600795</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -684,17 +684,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>743945</t>
+          <t>750471</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>23665</t>
+          <t>23850</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>615457</t>
+          <t>621521</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -715,17 +715,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>684113</t>
+          <t>688954</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>72179</t>
+          <t>72803</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>488416</t>
+          <t>492192</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -746,17 +746,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>655572</t>
+          <t>657627</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>15772</t>
+          <t>15857</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>585303</t>
+          <t>586844</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -808,12 +808,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>601700</t>
+          <t>613645</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>12460</t>
+          <t>12656</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -839,17 +839,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>442827</t>
+          <t>444674</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>12199</t>
+          <t>12254</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>415981</t>
+          <t>418101</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -880,7 +880,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>90840</t>
+          <t>91574</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -901,22 +901,22 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>416198</t>
+          <t>419043</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>23952</t>
+          <t>24118</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>355505</t>
+          <t>357632</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>[32]</t>
+          <t>[32][33]</t>
         </is>
       </c>
     </row>
@@ -932,12 +932,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>385936</t>
+          <t>390358</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>41732</t>
+          <t>41759</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -947,7 +947,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>[34]</t>
+          <t>[35]</t>
         </is>
       </c>
     </row>
@@ -963,22 +963,22 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>345805</t>
+          <t>347372</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>4881</t>
+          <t>4913</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>252335</t>
+          <t>254386</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>[35][36]</t>
+          <t>[36][37]</t>
         </is>
       </c>
     </row>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>[37]</t>
+          <t>[38]</t>
         </is>
       </c>
     </row>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>[38]</t>
+          <t>[39]</t>
         </is>
       </c>
     </row>
@@ -1056,22 +1056,22 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>304386</t>
+          <t>305031</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>6408</t>
+          <t>6415</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>291683</t>
+          <t>292044</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>[39]</t>
+          <t>[40]</t>
         </is>
       </c>
     </row>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>[40]</t>
+          <t>[41]</t>
         </is>
       </c>
     </row>
@@ -1118,22 +1118,22 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>293025</t>
+          <t>294932</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>35658</t>
+          <t>35668</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>215954</t>
+          <t>216807</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>[41]</t>
+          <t>[42]</t>
         </is>
       </c>
     </row>
@@ -1149,22 +1149,22 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>279526</t>
+          <t>283460</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4830</t>
+          <t>4930</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>208790</t>
+          <t>209885</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>[42][43]</t>
+          <t>[43][44]</t>
         </is>
       </c>
     </row>
@@ -1180,22 +1180,22 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>268418</t>
+          <t>271244</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>9452</t>
+          <t>9464</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>237311</t>
+          <t>238681</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>[45][44]</t>
+          <t>[46][45]</t>
         </is>
       </c>
     </row>
@@ -1211,22 +1211,22 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>236519</t>
+          <t>240687</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>9336</t>
+          <t>9448</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>170774</t>
+          <t>174350</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>[46]</t>
+          <t>[47]</t>
         </is>
       </c>
     </row>
@@ -1242,22 +1242,22 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>175256</t>
+          <t>179071</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1169</t>
+          <t>1196</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>126329</t>
+          <t>130024</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>[47]</t>
+          <t>[48]</t>
         </is>
       </c>
     </row>
@@ -1273,22 +1273,22 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>169472</t>
+          <t>172712</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>3468</t>
+          <t>3516</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>75486</t>
+          <t>76754</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>[48][49]</t>
+          <t>[49][50]</t>
         </is>
       </c>
     </row>
@@ -1304,22 +1304,22 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>140539</t>
+          <t>141911</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>9199</t>
+          <t>9205</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>122836</t>
+          <t>123723</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>[52]</t>
+          <t>[53]</t>
         </is>
       </c>
     </row>
@@ -1335,22 +1335,22 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>129419</t>
+          <t>130051</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>7511</t>
+          <t>7550</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>87716</t>
+          <t>88457</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>[53]</t>
+          <t>[54]</t>
         </is>
       </c>
     </row>
@@ -1361,27 +1361,27 @@
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Qatar</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>122917</t>
+          <t>124129</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>11044</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>119822</t>
+          <t>97063</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>[54]</t>
+          <t>[55][56]</t>
         </is>
       </c>
     </row>
@@ -1392,27 +1392,27 @@
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Qatar</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>122257</t>
+          <t>123146</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>11029</t>
+          <t>209</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>97063</t>
+          <t>120089</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>[55][56]</t>
+          <t>[57]</t>
         </is>
       </c>
     </row>
@@ -1428,22 +1428,22 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>110217</t>
+          <t>111550</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>4360</t>
+          <t>4402</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>88235</t>
+          <t>89119</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>[58][59]</t>
+          <t>[59][60]</t>
         </is>
       </c>
     </row>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>107056</t>
+          <t>107134</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1469,12 +1469,12 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>101455</t>
+          <t>101610</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>[60][61]</t>
+          <t>[61][62]</t>
         </is>
       </c>
     </row>
@@ -1490,22 +1490,22 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>106136</t>
+          <t>106732</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2034</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>79363</t>
+          <t>80179</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>[62]</t>
+          <t>[63]</t>
         </is>
       </c>
     </row>
@@ -1521,22 +1521,22 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>104138</t>
+          <t>104879</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2213</t>
+          <t>2229</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>77881</t>
+          <t>79093</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>[63]</t>
+          <t>[64]</t>
         </is>
       </c>
     </row>
@@ -1552,22 +1552,22 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>101641</t>
+          <t>101772</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>5715</t>
+          <t>5733</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>87158</t>
+          <t>87958</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>[64]</t>
+          <t>[65]</t>
         </is>
       </c>
     </row>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>[65]</t>
+          <t>[66]</t>
         </is>
       </c>
     </row>
@@ -1614,12 +1614,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>95948</t>
+          <t>97976</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>9935</t>
+          <t>9936</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1629,7 +1629,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>[67][68]</t>
+          <t>[68][69]</t>
         </is>
       </c>
     </row>
@@ -1645,22 +1645,22 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>94504</t>
+          <t>97264</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1714</t>
+          <t>1755</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>74930</t>
+          <t>76690</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>[70]</t>
+          <t>[71]</t>
         </is>
       </c>
     </row>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>[71]</t>
+          <t>[72]</t>
         </is>
       </c>
     </row>
@@ -1702,17 +1702,17 @@
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Netherlands[v]</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>88237</t>
+          <t>90047</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>5865</t>
+          <t>6273</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1722,7 +1722,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>[72]</t>
+          <t>[74][75]</t>
         </is>
       </c>
     </row>
@@ -1733,17 +1733,17 @@
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Netherlands[v]</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>88073</t>
+          <t>88237</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>6266</t>
+          <t>5865</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>[74][75]</t>
+          <t>[76]</t>
         </is>
       </c>
     </row>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>85255</t>
+          <t>85269</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1779,12 +1779,12 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>80456</t>
+          <t>80464</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>[76]</t>
+          <t>[77]</t>
         </is>
       </c>
     </row>
@@ -1800,22 +1800,22 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>83664</t>
+          <t>84344</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>3036</t>
+          <t>3076</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>73260</t>
+          <t>73748</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>[77]</t>
+          <t>[78]</t>
         </is>
       </c>
     </row>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>[78]</t>
+          <t>[79]</t>
         </is>
       </c>
     </row>
@@ -1857,27 +1857,27 @@
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Japan[x]</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>77494</t>
+          <t>78330</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1482</t>
+          <t>2282</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>69899</t>
+          <t>63861</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>[79]</t>
+          <t>[80][81]</t>
         </is>
       </c>
     </row>
@@ -1888,27 +1888,27 @@
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Japan[x]</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>77328</t>
+          <t>78073</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2270</t>
+          <t>1495</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>63312</t>
+          <t>70495</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>[80][81]</t>
+          <t>[82]</t>
         </is>
       </c>
     </row>
@@ -1924,22 +1924,22 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>75230</t>
+          <t>75461</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>773</t>
+          <t>776</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>73098</t>
+          <t>73212</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>[82]</t>
+          <t>[83]</t>
         </is>
       </c>
     </row>
@@ -1955,22 +1955,22 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>70120</t>
+          <t>70611</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2122</t>
+          <t>2146</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>20677</t>
+          <t>21149</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>[83][84]</t>
+          <t>[84][85]</t>
         </is>
       </c>
     </row>
@@ -1981,27 +1981,27 @@
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Ethiopia</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>67176</t>
+          <t>67515</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1894</t>
+          <t>1072</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>45053</t>
+          <t>27638</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>[85][86]</t>
+          <t>[86]</t>
         </is>
       </c>
     </row>
@@ -2012,27 +2012,27 @@
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Ethiopia</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>66913</t>
+          <t>67176</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1060</t>
+          <t>1894</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>27085</t>
+          <t>45053</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>[87]</t>
+          <t>[87][88]</t>
         </is>
       </c>
     </row>
@@ -2063,7 +2063,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>[88]</t>
+          <t>[89]</t>
         </is>
       </c>
     </row>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>[89]</t>
+          <t>[90]</t>
         </is>
       </c>
     </row>
@@ -2105,27 +2105,27 @@
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Nepal</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>61593</t>
+          <t>62374</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>390</t>
+          <t>686</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>43820</t>
+          <t>23160</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>[90]</t>
+          <t>[91]</t>
         </is>
       </c>
     </row>
@@ -2136,27 +2136,27 @@
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Nepal</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>60618</t>
+          <t>62797</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>666</t>
+          <t>401</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>22662</t>
+          <t>45267</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>[91]</t>
+          <t>[92]</t>
         </is>
       </c>
     </row>
@@ -2187,7 +2187,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>[92][93]</t>
+          <t>[93][94]</t>
         </is>
       </c>
     </row>
@@ -2203,22 +2203,22 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>56735</t>
+          <t>56935</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1093</t>
+          <t>1094</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>48092</t>
+          <t>48305</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>[94]</t>
+          <t>[95]</t>
         </is>
       </c>
     </row>
@@ -2249,7 +2249,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>[95]</t>
+          <t>[96]</t>
         </is>
       </c>
     </row>
@@ -2280,7 +2280,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>[96][97]</t>
+          <t>[97][98]</t>
         </is>
       </c>
     </row>
@@ -2311,7 +2311,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>[98][99]</t>
+          <t>[99][100]</t>
         </is>
       </c>
     </row>
@@ -2342,7 +2342,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>[100]</t>
+          <t>[101]</t>
         </is>
       </c>
     </row>
@@ -2353,27 +2353,27 @@
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Ghana</t>
+          <t>Moldova[z]</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>45714</t>
+          <t>46336</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>294</t>
+          <t>1201</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>44896</t>
+          <t>34236</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>[101]</t>
+          <t>[102]</t>
         </is>
       </c>
     </row>
@@ -2384,27 +2384,27 @@
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Moldova[z]</t>
+          <t>Ghana</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>45648</t>
+          <t>45877</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1186</t>
+          <t>297</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>33734</t>
+          <t>45081</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>[102]</t>
+          <t>[103]</t>
         </is>
       </c>
     </row>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>[103]</t>
+          <t>[104]</t>
         </is>
       </c>
     </row>
@@ -2466,7 +2466,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>[104]</t>
+          <t>[105]</t>
         </is>
       </c>
     </row>
@@ -2477,27 +2477,27 @@
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Azerbaijan[aa]</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>38872</t>
+          <t>39042</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1436</t>
+          <t>574</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>32505</t>
+          <t>36601</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>[105]</t>
+          <t>[106]</t>
         </is>
       </c>
     </row>
@@ -2508,27 +2508,27 @@
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Azerbaijan[aa]</t>
+          <t>Afghanistan</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>38777</t>
+          <t>38872</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>571</t>
+          <t>1436</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>36281</t>
+          <t>32505</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>[106]</t>
+          <t>[107]</t>
         </is>
       </c>
     </row>
@@ -2544,22 +2544,22 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>36661</t>
+          <t>37474</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>763</t>
+          <t>765</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>28451</t>
+          <t>28961</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>[107]</t>
+          <t>[108]</t>
         </is>
       </c>
     </row>
@@ -2590,7 +2590,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>[108]</t>
+          <t>[109]</t>
         </is>
       </c>
     </row>
@@ -2621,7 +2621,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>[109]</t>
+          <t>[110]</t>
         </is>
       </c>
     </row>
@@ -2637,12 +2637,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>32757</t>
+          <t>32840</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>739</t>
+          <t>740</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -2652,7 +2652,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>[110]</t>
+          <t>[111]</t>
         </is>
       </c>
     </row>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>[111]</t>
+          <t>[112]</t>
         </is>
       </c>
     </row>
@@ -2699,22 +2699,22 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>31113</t>
+          <t>32127</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>584</t>
+          <t>611</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>16313</t>
+          <t>16921</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>[112]</t>
+          <t>[113]</t>
         </is>
       </c>
     </row>
@@ -2730,22 +2730,22 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>27346</t>
+          <t>27428</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>804</t>
+          <t>808</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>20825</t>
+          <t>21247</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>[113]</t>
+          <t>[114]</t>
         </is>
       </c>
     </row>
@@ -2761,22 +2761,22 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>26861</t>
+          <t>26885</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>837</t>
+          <t>844</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>23850</t>
+          <t>23957</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>[114]</t>
+          <t>[115]</t>
         </is>
       </c>
     </row>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>[115]</t>
+          <t>[116]</t>
         </is>
       </c>
     </row>
@@ -2823,22 +2823,22 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>25822</t>
+          <t>26438</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>409</t>
+          <t>422</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>13908</t>
+          <t>14207</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>[116][117]</t>
+          <t>[117][118]</t>
         </is>
       </c>
     </row>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>[118]</t>
+          <t>[119]</t>
         </is>
       </c>
     </row>
@@ -2885,22 +2885,22 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>22783</t>
+          <t>22893</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>377</t>
+          <t>378</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>19771</t>
+          <t>19970</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>[119][120]</t>
+          <t>[120][121]</t>
         </is>
       </c>
     </row>
@@ -2931,7 +2931,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>[121][122]</t>
+          <t>[122][123]</t>
         </is>
       </c>
     </row>
@@ -2962,7 +2962,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>[123][124]</t>
+          <t>[124][125]</t>
         </is>
       </c>
     </row>
@@ -2993,7 +2993,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>[125]</t>
+          <t>[126]</t>
         </is>
       </c>
     </row>
@@ -3024,7 +3024,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>[126][127]</t>
+          <t>[127][128]</t>
         </is>
       </c>
     </row>
@@ -3055,7 +3055,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>[128][129]</t>
+          <t>[129][130]</t>
         </is>
       </c>
     </row>
@@ -3066,27 +3066,27 @@
       <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr">
         <is>
-          <t>North Macedonia</t>
+          <t>Hungary</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>16417</t>
+          <t>16920</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>683</t>
+          <t>675</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>13732</t>
+          <t>4382</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>[130][131]</t>
+          <t>[131]</t>
         </is>
       </c>
     </row>
@@ -3097,27 +3097,27 @@
       <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Madagascar</t>
+          <t>North Macedonia</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>15871</t>
+          <t>16417</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>683</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>14482</t>
+          <t>13732</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>[132]</t>
+          <t>[132][133]</t>
         </is>
       </c>
     </row>
@@ -3128,27 +3128,27 @@
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Kosovo</t>
+          <t>Madagascar</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>14839</t>
+          <t>15871</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>601</t>
+          <t>215</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>11784</t>
+          <t>14482</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>[133][134]</t>
+          <t>[134]</t>
         </is>
       </c>
     </row>
@@ -3159,27 +3159,27 @@
       <c r="B89" t="inlineStr"/>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Senegal</t>
+          <t>Kosovo</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>14529</t>
+          <t>14839</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>298</t>
+          <t>601</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>10692</t>
+          <t>11784</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>[135]</t>
+          <t>[135][136]</t>
         </is>
       </c>
     </row>
@@ -3190,27 +3190,27 @@
       <c r="B90" t="inlineStr"/>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Hungary</t>
+          <t>Croatia</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>16111</t>
+          <t>14725</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>669</t>
+          <t>244</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>4240</t>
+          <t>12353</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>[136]</t>
+          <t>[137]</t>
         </is>
       </c>
     </row>
@@ -3221,27 +3221,27 @@
       <c r="B91" t="inlineStr"/>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Croatia</t>
+          <t>Senegal</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>14513</t>
+          <t>14688</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>244</t>
+          <t>302</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>12169</t>
+          <t>11153</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>[137]</t>
+          <t>[138]</t>
         </is>
       </c>
     </row>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>[138][139]</t>
+          <t>[139][140]</t>
         </is>
       </c>
     </row>
@@ -3303,7 +3303,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>[140]</t>
+          <t>[141]</t>
         </is>
       </c>
     </row>
@@ -3334,7 +3334,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>[141][142]</t>
+          <t>[142][143]</t>
         </is>
       </c>
     </row>
@@ -3350,7 +3350,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>12708</t>
+          <t>12769</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -3365,7 +3365,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>[145]</t>
+          <t>[146]</t>
         </is>
       </c>
     </row>
@@ -3396,7 +3396,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>[146][147]</t>
+          <t>[147][148]</t>
         </is>
       </c>
     </row>
@@ -3412,7 +3412,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>10456</t>
+          <t>10488</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -3422,12 +3422,12 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>9863</t>
+          <t>9891</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>[148]</t>
+          <t>[149]</t>
         </is>
       </c>
     </row>
@@ -3443,22 +3443,22 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>10207</t>
+          <t>10292</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>111</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>7947</t>
+          <t>7969</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>[149]</t>
+          <t>[150]</t>
         </is>
       </c>
     </row>
@@ -3474,22 +3474,22 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>10147</t>
+          <t>10167</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>129</t>
+          <t>130</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>9264</t>
+          <t>9315</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>[150]</t>
+          <t>[151]</t>
         </is>
       </c>
     </row>
@@ -3520,7 +3520,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>[151][152]</t>
+          <t>[152][153]</t>
         </is>
       </c>
     </row>
@@ -3536,7 +3536,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>9494</t>
+          <t>9568</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -3546,12 +3546,12 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>7990</t>
+          <t>8068</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>[153]</t>
+          <t>[154]</t>
         </is>
       </c>
     </row>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>[154]</t>
+          <t>[155]</t>
         </is>
       </c>
     </row>
@@ -3598,12 +3598,12 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>8858</t>
+          <t>8922</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>337</t>
+          <t>339</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -3613,7 +3613,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>[157]</t>
+          <t>[158]</t>
         </is>
       </c>
     </row>
@@ -3644,7 +3644,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>[158]</t>
+          <t>[159]</t>
         </is>
       </c>
     </row>
@@ -3655,27 +3655,27 @@
       <c r="B105" t="inlineStr"/>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Tunisia</t>
+          <t>Haiti</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>8570</t>
+          <t>8600</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>221</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>2342</t>
+          <t>6363</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>[159]</t>
+          <t>[160]</t>
         </is>
       </c>
     </row>
@@ -3686,27 +3686,27 @@
       <c r="B106" t="inlineStr"/>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Haiti</t>
+          <t>Tunisia</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>8556</t>
+          <t>8570</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>133</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>6315</t>
+          <t>2342</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>[160]</t>
+          <t>[161]</t>
         </is>
       </c>
     </row>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>[161]</t>
+          <t>[162]</t>
         </is>
       </c>
     </row>
@@ -3768,7 +3768,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>[162]</t>
+          <t>[163]</t>
         </is>
       </c>
     </row>
@@ -3799,7 +3799,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>[163]</t>
+          <t>[164]</t>
         </is>
       </c>
     </row>
@@ -3830,7 +3830,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>[164]</t>
+          <t>[165]</t>
         </is>
       </c>
     </row>
@@ -3861,7 +3861,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>[165]</t>
+          <t>[166]</t>
         </is>
       </c>
     </row>
@@ -3892,7 +3892,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>[166]</t>
+          <t>[167]</t>
         </is>
       </c>
     </row>
@@ -3908,7 +3908,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>5711</t>
+          <t>5716</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -3918,12 +3918,12 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>4000</t>
+          <t>4026</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>[167]</t>
+          <t>[168]</t>
         </is>
       </c>
     </row>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>[168]</t>
+          <t>[169]</t>
         </is>
       </c>
     </row>
@@ -3985,7 +3985,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>[169]</t>
+          <t>[170]</t>
         </is>
       </c>
     </row>
@@ -3996,27 +3996,27 @@
       <c r="B116" t="inlineStr"/>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Uganda</t>
+          <t>Cape Verde</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>5123</t>
+          <t>5141</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>50</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>2333</t>
+          <t>4548</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>[170][171]</t>
+          <t>[171]</t>
         </is>
       </c>
     </row>
@@ -4027,27 +4027,27 @@
       <c r="B117" t="inlineStr"/>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Cape Verde</t>
+          <t>Uganda</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>5063</t>
+          <t>5123</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>58</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>4465</t>
+          <t>2333</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>[172]</t>
+          <t>[172][173]</t>
         </is>
       </c>
     </row>
@@ -4058,27 +4058,27 @@
       <c r="B118" t="inlineStr"/>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Cuba[ah]</t>
+          <t>Hong Kong</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>5004</t>
+          <t>5010</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>111</t>
+          <t>103</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>4249</t>
+          <t>4707</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>[173]</t>
+          <t>[174]</t>
         </is>
       </c>
     </row>
@@ -4089,27 +4089,27 @@
       <c r="B119" t="inlineStr"/>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Equatorial Guinea</t>
+          <t>Cuba[ah]</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>5000</t>
+          <t>5004</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>111</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>4496</t>
+          <t>4249</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>[174]</t>
+          <t>[175]</t>
         </is>
       </c>
     </row>
@@ -4120,27 +4120,27 @@
       <c r="B120" t="inlineStr"/>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Hong Kong</t>
+          <t>Equatorial Guinea</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>4997</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>4696</t>
+          <t>4496</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>[175]</t>
+          <t>[176]</t>
         </is>
       </c>
     </row>
@@ -4171,7 +4171,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>[176][177]</t>
+          <t>[177][178]</t>
         </is>
       </c>
     </row>
@@ -4202,7 +4202,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>[80][178]</t>
+          <t>[80][179]</t>
         </is>
       </c>
     </row>
@@ -4233,7 +4233,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>[179]</t>
+          <t>[180]</t>
         </is>
       </c>
     </row>
@@ -4249,22 +4249,22 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>4671</t>
+          <t>4691</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>96</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>4160</t>
+          <t>4280</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>[180]</t>
+          <t>[181]</t>
         </is>
       </c>
     </row>
@@ -4295,7 +4295,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>[181][182]</t>
+          <t>[182][183]</t>
         </is>
       </c>
     </row>
@@ -4311,12 +4311,12 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>4467</t>
+          <t>4621</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -4326,7 +4326,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>[183]</t>
+          <t>[184]</t>
         </is>
       </c>
     </row>
@@ -4342,22 +4342,22 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>4358</t>
+          <t>4556</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>55</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>1225</t>
+          <t>1264</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>[184][185]</t>
+          <t>[185][186]</t>
         </is>
       </c>
     </row>
@@ -4388,7 +4388,7 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>[186]</t>
+          <t>[187]</t>
         </is>
       </c>
     </row>
@@ -4419,7 +4419,7 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>[187][188]</t>
+          <t>[188][189]</t>
         </is>
       </c>
     </row>
@@ -4430,27 +4430,27 @@
       <c r="B130" t="inlineStr"/>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Syria[aj]</t>
+          <t>Lithuania</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>3614</t>
+          <t>3664</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>87</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>871</t>
+          <t>2197</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>[189]</t>
+          <t>[190][191]</t>
         </is>
       </c>
     </row>
@@ -4461,27 +4461,27 @@
       <c r="B131" t="inlineStr"/>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Angola</t>
+          <t>Trinidad and Tobago</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>3569</t>
+          <t>3651</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>60</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>1332</t>
+          <t>822</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>[190]</t>
+          <t>[192][193]</t>
         </is>
       </c>
     </row>
@@ -4492,27 +4492,27 @@
       <c r="B132" t="inlineStr"/>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Lithuania</t>
+          <t>Syria[aj]</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>3504</t>
+          <t>3614</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>160</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>2149</t>
+          <t>871</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>[191][192]</t>
+          <t>[194]</t>
         </is>
       </c>
     </row>
@@ -4523,27 +4523,27 @@
       <c r="B133" t="inlineStr"/>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>Angola</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>3497</t>
+          <t>3569</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>139</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>3328</t>
+          <t>1332</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>[193][194]</t>
+          <t>[195]</t>
         </is>
       </c>
     </row>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>3485</t>
+          <t>3504</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -4569,12 +4569,12 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>1973</t>
+          <t>19992</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>[195]</t>
+          <t>[196]</t>
         </is>
       </c>
     </row>
@@ -4585,27 +4585,27 @@
       <c r="B135" t="inlineStr"/>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Aruba</t>
+          <t>Thailand</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>3460</t>
+          <t>3500</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>59</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>2128</t>
+          <t>3338</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>[196]</t>
+          <t>[197][198]</t>
         </is>
       </c>
     </row>
@@ -4616,27 +4616,27 @@
       <c r="B136" t="inlineStr"/>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Trinidad and Tobago</t>
+          <t>Aruba</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>3434</t>
+          <t>3460</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>23</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>814</t>
+          <t>2128</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>[197][198]</t>
+          <t>[199]</t>
         </is>
       </c>
     </row>
@@ -4667,7 +4667,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>[199]</t>
+          <t>[200]</t>
         </is>
       </c>
     </row>
@@ -4678,27 +4678,27 @@
       <c r="B138" t="inlineStr"/>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Sri Lanka</t>
+          <t>Georgia[al]</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>3281</t>
+          <t>3306</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>3060</t>
+          <t>1481</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>[200]</t>
+          <t>[201]</t>
         </is>
       </c>
     </row>
@@ -4709,27 +4709,27 @@
       <c r="B139" t="inlineStr"/>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Bahamas[al]</t>
+          <t>Sri Lanka</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>3177</t>
+          <t>3281</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>1626</t>
+          <t>3070</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>[201][202]</t>
+          <t>[202]</t>
         </is>
       </c>
     </row>
@@ -4740,27 +4740,27 @@
       <c r="B140" t="inlineStr"/>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Georgia[am]</t>
+          <t>Bahamas[am]</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>3119</t>
+          <t>3177</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>69</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>1435</t>
+          <t>1626</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>[203]</t>
+          <t>[203][204]</t>
         </is>
       </c>
     </row>
@@ -4791,7 +4791,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>[204]</t>
+          <t>[205]</t>
         </is>
       </c>
     </row>
@@ -4822,7 +4822,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>[205]</t>
+          <t>[206]</t>
         </is>
       </c>
     </row>
@@ -4853,7 +4853,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>[206][207]</t>
+          <t>[207][208]</t>
         </is>
       </c>
     </row>
@@ -4884,7 +4884,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>[208]</t>
+          <t>[209]</t>
         </is>
       </c>
     </row>
@@ -4915,7 +4915,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>[209][210]</t>
+          <t>[210][211]</t>
         </is>
       </c>
     </row>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>[211]</t>
+          <t>[212]</t>
         </is>
       </c>
     </row>
@@ -4977,7 +4977,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>[212][213]</t>
+          <t>[213][214]</t>
         </is>
       </c>
     </row>
@@ -4993,7 +4993,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>2230</t>
+          <t>2307</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
@@ -5003,12 +5003,12 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>2112</t>
+          <t>2116</t>
         </is>
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>[214]</t>
+          <t>[215]</t>
         </is>
       </c>
     </row>
@@ -5039,7 +5039,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>[215][216]</t>
+          <t>[216][217]</t>
         </is>
       </c>
     </row>
@@ -5055,12 +5055,12 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>2027</t>
+          <t>2102</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>64</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -5070,7 +5070,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>[217]</t>
+          <t>[218][219]</t>
         </is>
       </c>
     </row>
@@ -5101,7 +5101,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>[218]</t>
+          <t>[220]</t>
         </is>
       </c>
     </row>
@@ -5132,7 +5132,7 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>[9][219]</t>
+          <t>[9][221]</t>
         </is>
       </c>
     </row>
@@ -5148,7 +5148,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>1876</t>
+          <t>1890</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -5158,12 +5158,12 @@
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>1582</t>
+          <t>1603</t>
         </is>
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>[220]</t>
+          <t>[222]</t>
         </is>
       </c>
     </row>
@@ -5179,22 +5179,22 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>1618</t>
+          <t>1640</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>41</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>1243</t>
+          <t>1251</t>
         </is>
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>[221]</t>
+          <t>[223]</t>
         </is>
       </c>
     </row>
@@ -5225,7 +5225,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>[222]</t>
+          <t>[224]</t>
         </is>
       </c>
     </row>
@@ -5256,7 +5256,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>[223]</t>
+          <t>[225]</t>
         </is>
       </c>
     </row>
@@ -5272,7 +5272,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>1498</t>
+          <t>1515</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
@@ -5287,7 +5287,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>[80][224]</t>
+          <t>[80][226]</t>
         </is>
       </c>
     </row>
@@ -5303,7 +5303,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>1458</t>
+          <t>1460</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
@@ -5313,12 +5313,12 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>1363</t>
+          <t>1368</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>[225]</t>
+          <t>[227]</t>
         </is>
       </c>
     </row>
@@ -5349,7 +5349,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>[226][227]</t>
+          <t>[228][229]</t>
         </is>
       </c>
     </row>
@@ -5380,7 +5380,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>[228]</t>
+          <t>[230]</t>
         </is>
       </c>
     </row>
@@ -5411,7 +5411,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>[229][230]</t>
+          <t>[231][232]</t>
         </is>
       </c>
     </row>
@@ -5442,7 +5442,7 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>[231]</t>
+          <t>[233]</t>
         </is>
       </c>
     </row>
@@ -5473,7 +5473,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>[232]</t>
+          <t>[234]</t>
         </is>
       </c>
     </row>
@@ -5504,7 +5504,7 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>[233]</t>
+          <t>[235]</t>
         </is>
       </c>
     </row>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>[234]</t>
+          <t>[236]</t>
         </is>
       </c>
     </row>
@@ -5566,7 +5566,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>[235][236]</t>
+          <t>[237][238]</t>
         </is>
       </c>
     </row>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>[237]</t>
+          <t>[239]</t>
         </is>
       </c>
     </row>
@@ -5628,7 +5628,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>[238]</t>
+          <t>[240]</t>
         </is>
       </c>
     </row>
@@ -5659,7 +5659,7 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>[242]</t>
+          <t>[244]</t>
         </is>
       </c>
     </row>
@@ -5690,7 +5690,7 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>[243]</t>
+          <t>[245]</t>
         </is>
       </c>
     </row>
@@ -5721,7 +5721,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>[244]</t>
+          <t>[246]</t>
         </is>
       </c>
     </row>
@@ -5752,7 +5752,7 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>[245][246]</t>
+          <t>[247][248]</t>
         </is>
       </c>
     </row>
@@ -5783,7 +5783,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>[247]</t>
+          <t>[249]</t>
         </is>
       </c>
     </row>
@@ -5814,7 +5814,7 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>[248]</t>
+          <t>[250]</t>
         </is>
       </c>
     </row>
@@ -5845,7 +5845,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>[249][250]</t>
+          <t>[251][252]</t>
         </is>
       </c>
     </row>
@@ -5876,7 +5876,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>[251][252]</t>
+          <t>[253][254]</t>
         </is>
       </c>
     </row>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>[253]</t>
+          <t>[255]</t>
         </is>
       </c>
     </row>
@@ -5923,7 +5923,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>663</t>
+          <t>667</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
@@ -5933,12 +5933,12 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>566</t>
+          <t>568</t>
         </is>
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>[254]</t>
+          <t>[256]</t>
         </is>
       </c>
     </row>
@@ -5954,22 +5954,22 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>565</t>
+          <t>574</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>477</t>
+          <t>488</t>
         </is>
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>[255]</t>
+          <t>[257]</t>
         </is>
       </c>
     </row>
@@ -6000,7 +6000,7 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>[256]</t>
+          <t>[258]</t>
         </is>
       </c>
     </row>
@@ -6016,7 +6016,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>503</t>
+          <t>506</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
@@ -6026,12 +6026,12 @@
       </c>
       <c r="F181" t="inlineStr">
         <is>
-          <t>478</t>
+          <t>479</t>
         </is>
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>[258]</t>
+          <t>[260]</t>
         </is>
       </c>
     </row>
@@ -6062,7 +6062,7 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>[259]</t>
+          <t>[261]</t>
         </is>
       </c>
     </row>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>[260]</t>
+          <t>[262]</t>
         </is>
       </c>
     </row>
@@ -6124,7 +6124,7 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>[261][262]</t>
+          <t>[263][264]</t>
         </is>
       </c>
     </row>
@@ -6155,7 +6155,7 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>[263]</t>
+          <t>[265]</t>
         </is>
       </c>
     </row>
@@ -6186,7 +6186,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>[264]</t>
+          <t>[266]</t>
         </is>
       </c>
     </row>
@@ -6217,7 +6217,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>[265]</t>
+          <t>[267]</t>
         </is>
       </c>
     </row>
@@ -6248,7 +6248,7 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>[266]</t>
+          <t>[268]</t>
         </is>
       </c>
     </row>
@@ -6279,7 +6279,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>[251][267]</t>
+          <t>[253][269]</t>
         </is>
       </c>
     </row>
@@ -6310,7 +6310,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>[268]</t>
+          <t>[270]</t>
         </is>
       </c>
     </row>
@@ -6341,7 +6341,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>[269]</t>
+          <t>[271]</t>
         </is>
       </c>
     </row>
@@ -6372,7 +6372,7 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>[270]</t>
+          <t>[272]</t>
         </is>
       </c>
     </row>
@@ -6383,27 +6383,27 @@
       <c r="B193" t="inlineStr"/>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Guernsey</t>
+          <t>Bhutan</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>254</t>
+          <t>258</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>239</t>
+          <t>186</t>
         </is>
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>[271]</t>
+          <t>[273]</t>
         </is>
       </c>
     </row>
@@ -6414,27 +6414,27 @@
       <c r="B194" t="inlineStr"/>
       <c r="C194" t="inlineStr">
         <is>
-          <t>Bhutan</t>
+          <t>Guernsey</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>252</t>
+          <t>254</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>239</t>
         </is>
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>[272]</t>
+          <t>[274]</t>
         </is>
       </c>
     </row>
@@ -6450,7 +6450,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>228</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
@@ -6460,12 +6460,12 @@
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t>74</t>
+          <t>83</t>
         </is>
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>[273]</t>
+          <t>[275]</t>
         </is>
       </c>
     </row>
@@ -6496,7 +6496,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>[274]</t>
+          <t>[276]</t>
         </is>
       </c>
     </row>
@@ -6527,7 +6527,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>[275]</t>
+          <t>[277]</t>
         </is>
       </c>
     </row>
@@ -6558,7 +6558,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>[276]</t>
+          <t>[278]</t>
         </is>
       </c>
     </row>
@@ -6589,7 +6589,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>[277]</t>
+          <t>[279]</t>
         </is>
       </c>
     </row>
@@ -6620,7 +6620,7 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>[278][279]</t>
+          <t>[280][281]</t>
         </is>
       </c>
     </row>
@@ -6651,7 +6651,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>[280][281]</t>
+          <t>[282][283]</t>
         </is>
       </c>
     </row>
@@ -6682,7 +6682,7 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>[282]</t>
+          <t>[284]</t>
         </is>
       </c>
     </row>
@@ -6713,7 +6713,7 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>[283][284]</t>
+          <t>[285][286]</t>
         </is>
       </c>
     </row>
@@ -6744,7 +6744,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>[285]</t>
+          <t>[287]</t>
         </is>
       </c>
     </row>
@@ -6775,7 +6775,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>[286][287]</t>
+          <t>[288][289]</t>
         </is>
       </c>
     </row>
@@ -6806,7 +6806,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>[251]</t>
+          <t>[253]</t>
         </is>
       </c>
     </row>
@@ -6837,7 +6837,7 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>[288]</t>
+          <t>[290]</t>
         </is>
       </c>
     </row>
@@ -6868,7 +6868,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>[289][290]</t>
+          <t>[291][292]</t>
         </is>
       </c>
     </row>
@@ -6899,7 +6899,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>[291]</t>
+          <t>[293]</t>
         </is>
       </c>
     </row>
@@ -6930,7 +6930,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>[292]</t>
+          <t>[294]</t>
         </is>
       </c>
     </row>
@@ -6961,7 +6961,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>[293]</t>
+          <t>[295]</t>
         </is>
       </c>
     </row>
@@ -6992,7 +6992,7 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>[294]</t>
+          <t>[296]</t>
         </is>
       </c>
     </row>
@@ -7023,7 +7023,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>[295][296]</t>
+          <t>[297][298]</t>
         </is>
       </c>
     </row>
@@ -7054,7 +7054,7 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>[297]</t>
+          <t>[299]</t>
         </is>
       </c>
     </row>
@@ -7085,7 +7085,7 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>[298][299]</t>
+          <t>[300][301]</t>
         </is>
       </c>
     </row>
@@ -7116,7 +7116,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>[300][301]</t>
+          <t>[302][303]</t>
         </is>
       </c>
     </row>
@@ -7147,7 +7147,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>[302]</t>
+          <t>[304]</t>
         </is>
       </c>
     </row>
@@ -7178,7 +7178,7 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>[303]</t>
+          <t>[305]</t>
         </is>
       </c>
     </row>
@@ -7209,7 +7209,7 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>[304]</t>
+          <t>[306]</t>
         </is>
       </c>
     </row>
@@ -7240,7 +7240,7 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>[305][306]</t>
+          <t>[307][308]</t>
         </is>
       </c>
     </row>
@@ -7271,7 +7271,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>[307]</t>
+          <t>[309]</t>
         </is>
       </c>
     </row>
@@ -7302,7 +7302,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>[308]</t>
+          <t>[310]</t>
         </is>
       </c>
     </row>
@@ -7333,7 +7333,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>[311][312]</t>
+          <t>[313][314]</t>
         </is>
       </c>
     </row>
@@ -7364,7 +7364,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>[314]</t>
+          <t>[316]</t>
         </is>
       </c>
     </row>
@@ -7395,7 +7395,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>[315]</t>
+          <t>[317]</t>
         </is>
       </c>
     </row>
@@ -7426,7 +7426,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>[316]</t>
+          <t>[318]</t>
         </is>
       </c>
     </row>
@@ -7457,7 +7457,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>[317][318]</t>
+          <t>[319][320]</t>
         </is>
       </c>
     </row>
@@ -7488,7 +7488,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>[319][322]</t>
+          <t>[321][324]</t>
         </is>
       </c>
     </row>
@@ -7519,7 +7519,7 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>[323]</t>
+          <t>[325]</t>
         </is>
       </c>
     </row>
@@ -7550,7 +7550,7 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>[324]</t>
+          <t>[326]</t>
         </is>
       </c>
     </row>
@@ -7581,7 +7581,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>[326][327]</t>
+          <t>[328][329]</t>
         </is>
       </c>
     </row>
@@ -7591,32 +7591,32 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>As of 18 September 2020 (UTC) · History of cases · History of deaths</t>
+          <t>As of 19 September 2020 (UTC) · History of cases · History of deaths</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>As of 18 September 2020 (UTC) · History of cases · History of deaths</t>
+          <t>As of 19 September 2020 (UTC) · History of cases · History of deaths</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>As of 18 September 2020 (UTC) · History of cases · History of deaths</t>
+          <t>As of 19 September 2020 (UTC) · History of cases · History of deaths</t>
         </is>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>As of 18 September 2020 (UTC) · History of cases · History of deaths</t>
+          <t>As of 19 September 2020 (UTC) · History of cases · History of deaths</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>As of 18 September 2020 (UTC) · History of cases · History of deaths</t>
+          <t>As of 19 September 2020 (UTC) · History of cases · History of deaths</t>
         </is>
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>As of 18 September 2020 (UTC) · History of cases · History of deaths</t>
+          <t>As of 19 September 2020 (UTC) · History of cases · History of deaths</t>
         </is>
       </c>
     </row>
@@ -7626,32 +7626,32 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reported to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations. ^ Deaths: Reporting criteria vary between locations. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations and some countries do not report recoveries. ^ The worldwide totals for cases, deaths and recoveries are taken from the John Hopkins University Coronavirus Resource Center. They are not sums of the figures for the listed countries and territories. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ SpainThe figure for cases excludes serology–confirmed cases.As of 19 May 2020, the Spanish government does not publish the number of recoveries. The last update on 18 May reported 150,376 recovered patients. ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[23] ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[26]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[27] In the latest report (11 September 2020), the number of total deaths is 16,165.[28] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[30]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[30] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[33] ^ GermanyNot all state authorities count recoveries.[44]Recoveries include estimations by the Robert Koch Institute.[44][45] ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[50] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[51] ^ RomaniaOn 18 September 2020, the large increase in the number of recoveries was a result of "the review and updating of data by the Ministry of Health and CNCCI".[57] ^ EgyptIncludes cases identified on the MS River Anuket. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[66] ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[69] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[73] ^ ChinaExcluding 366 asymptomatic cases under medical observation as of 17 September 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ MoldovaIncluding the disputed territory of Transnistria. ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[143] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[144] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[155] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[156] ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomaliaExcluding the de facto state of Somaliland. ^ Some of these deaths may still be under investigation as stated in the Ministry's press release. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana1,350 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[229] ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[238] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[239][240][241] ^ SomalilandCases from this de facto state are not counted by Somalia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ TaiwanIncluding cases from the ROCS Pan Shi.[257] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[268] ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[309][310]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[313]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[319]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[320][321] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[325] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[326][327]</t>
+          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reported to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations. ^ Deaths: Reporting criteria vary between locations. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations and some countries do not report recoveries. ^ The worldwide totals for cases, deaths and recoveries are taken from the John Hopkins University Coronavirus Resource Center. They are not sums of the figures for the listed countries and territories. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ SpainThe figure for cases excludes serology–confirmed cases.As of 19 May 2020, the Spanish government does not publish the number of recoveries. The last update on 18 May reported 150,376 recovered patients. ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[23] ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[26]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[27] In the latest report (11 September 2020), the number of total deaths is 16,165.[28] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[30]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[30] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[34] ^ GermanyNot all state authorities count recoveries.[45]Recoveries include estimations by the Robert Koch Institute.[45][46] ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[51] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[52] ^ RomaniaOn 18 September 2020, the large increase in the number of recoveries was a result of "the review and updating of data by the Ministry of Health and CNCCI".[58] ^ EgyptIncludes cases identified on the MS River Anuket. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[67] ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[70] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[73] ^ ChinaExcluding 374 asymptomatic cases under medical observation as of 18 September 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ MoldovaIncluding the disputed territory of Transnistria. ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[144] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[145] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[156] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[157] ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomaliaExcluding the de facto state of Somaliland. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ Some of these deaths may still be under investigation as stated in the Ministry's press release. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana1,350 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[231] ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[240] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[241][242][243] ^ SomalilandCases from this de facto state are not counted by Somalia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ TaiwanIncluding cases from the ROCS Pan Shi.[259] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[270] ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[311][312]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[315]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[321]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[322][323] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[327] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[328][329]</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reported to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations. ^ Deaths: Reporting criteria vary between locations. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations and some countries do not report recoveries. ^ The worldwide totals for cases, deaths and recoveries are taken from the John Hopkins University Coronavirus Resource Center. They are not sums of the figures for the listed countries and territories. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ SpainThe figure for cases excludes serology–confirmed cases.As of 19 May 2020, the Spanish government does not publish the number of recoveries. The last update on 18 May reported 150,376 recovered patients. ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[23] ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[26]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[27] In the latest report (11 September 2020), the number of total deaths is 16,165.[28] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[30]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[30] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[33] ^ GermanyNot all state authorities count recoveries.[44]Recoveries include estimations by the Robert Koch Institute.[44][45] ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[50] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[51] ^ RomaniaOn 18 September 2020, the large increase in the number of recoveries was a result of "the review and updating of data by the Ministry of Health and CNCCI".[57] ^ EgyptIncludes cases identified on the MS River Anuket. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[66] ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[69] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[73] ^ ChinaExcluding 366 asymptomatic cases under medical observation as of 17 September 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ MoldovaIncluding the disputed territory of Transnistria. ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[143] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[144] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[155] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[156] ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomaliaExcluding the de facto state of Somaliland. ^ Some of these deaths may still be under investigation as stated in the Ministry's press release. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana1,350 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[229] ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[238] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[239][240][241] ^ SomalilandCases from this de facto state are not counted by Somalia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ TaiwanIncluding cases from the ROCS Pan Shi.[257] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[268] ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[309][310]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[313]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[319]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[320][321] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[325] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[326][327]</t>
+          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reported to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations. ^ Deaths: Reporting criteria vary between locations. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations and some countries do not report recoveries. ^ The worldwide totals for cases, deaths and recoveries are taken from the John Hopkins University Coronavirus Resource Center. They are not sums of the figures for the listed countries and territories. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ SpainThe figure for cases excludes serology–confirmed cases.As of 19 May 2020, the Spanish government does not publish the number of recoveries. The last update on 18 May reported 150,376 recovered patients. ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[23] ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[26]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[27] In the latest report (11 September 2020), the number of total deaths is 16,165.[28] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[30]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[30] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[34] ^ GermanyNot all state authorities count recoveries.[45]Recoveries include estimations by the Robert Koch Institute.[45][46] ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[51] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[52] ^ RomaniaOn 18 September 2020, the large increase in the number of recoveries was a result of "the review and updating of data by the Ministry of Health and CNCCI".[58] ^ EgyptIncludes cases identified on the MS River Anuket. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[67] ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[70] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[73] ^ ChinaExcluding 374 asymptomatic cases under medical observation as of 18 September 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ MoldovaIncluding the disputed territory of Transnistria. ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[144] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[145] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[156] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[157] ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomaliaExcluding the de facto state of Somaliland. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ Some of these deaths may still be under investigation as stated in the Ministry's press release. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana1,350 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[231] ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[240] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[241][242][243] ^ SomalilandCases from this de facto state are not counted by Somalia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ TaiwanIncluding cases from the ROCS Pan Shi.[259] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[270] ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[311][312]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[315]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[321]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[322][323] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[327] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[328][329]</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reported to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations. ^ Deaths: Reporting criteria vary between locations. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations and some countries do not report recoveries. ^ The worldwide totals for cases, deaths and recoveries are taken from the John Hopkins University Coronavirus Resource Center. They are not sums of the figures for the listed countries and territories. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ SpainThe figure for cases excludes serology–confirmed cases.As of 19 May 2020, the Spanish government does not publish the number of recoveries. The last update on 18 May reported 150,376 recovered patients. ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[23] ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[26]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[27] In the latest report (11 September 2020), the number of total deaths is 16,165.[28] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[30]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[30] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[33] ^ GermanyNot all state authorities count recoveries.[44]Recoveries include estimations by the Robert Koch Institute.[44][45] ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[50] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[51] ^ RomaniaOn 18 September 2020, the large increase in the number of recoveries was a result of "the review and updating of data by the Ministry of Health and CNCCI".[57] ^ EgyptIncludes cases identified on the MS River Anuket. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[66] ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[69] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[73] ^ ChinaExcluding 366 asymptomatic cases under medical observation as of 17 September 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ MoldovaIncluding the disputed territory of Transnistria. ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[143] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[144] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[155] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[156] ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomaliaExcluding the de facto state of Somaliland. ^ Some of these deaths may still be under investigation as stated in the Ministry's press release. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana1,350 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[229] ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[238] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[239][240][241] ^ SomalilandCases from this de facto state are not counted by Somalia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ TaiwanIncluding cases from the ROCS Pan Shi.[257] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[268] ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[309][310]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[313]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[319]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[320][321] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[325] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[326][327]</t>
+          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reported to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations. ^ Deaths: Reporting criteria vary between locations. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations and some countries do not report recoveries. ^ The worldwide totals for cases, deaths and recoveries are taken from the John Hopkins University Coronavirus Resource Center. They are not sums of the figures for the listed countries and territories. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ SpainThe figure for cases excludes serology–confirmed cases.As of 19 May 2020, the Spanish government does not publish the number of recoveries. The last update on 18 May reported 150,376 recovered patients. ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[23] ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[26]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[27] In the latest report (11 September 2020), the number of total deaths is 16,165.[28] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[30]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[30] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[34] ^ GermanyNot all state authorities count recoveries.[45]Recoveries include estimations by the Robert Koch Institute.[45][46] ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[51] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[52] ^ RomaniaOn 18 September 2020, the large increase in the number of recoveries was a result of "the review and updating of data by the Ministry of Health and CNCCI".[58] ^ EgyptIncludes cases identified on the MS River Anuket. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[67] ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[70] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[73] ^ ChinaExcluding 374 asymptomatic cases under medical observation as of 18 September 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ MoldovaIncluding the disputed territory of Transnistria. ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[144] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[145] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[156] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[157] ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomaliaExcluding the de facto state of Somaliland. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ Some of these deaths may still be under investigation as stated in the Ministry's press release. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana1,350 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[231] ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[240] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[241][242][243] ^ SomalilandCases from this de facto state are not counted by Somalia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ TaiwanIncluding cases from the ROCS Pan Shi.[259] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[270] ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[311][312]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[315]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[321]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[322][323] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[327] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[328][329]</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reported to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations. ^ Deaths: Reporting criteria vary between locations. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations and some countries do not report recoveries. ^ The worldwide totals for cases, deaths and recoveries are taken from the John Hopkins University Coronavirus Resource Center. They are not sums of the figures for the listed countries and territories. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ SpainThe figure for cases excludes serology–confirmed cases.As of 19 May 2020, the Spanish government does not publish the number of recoveries. The last update on 18 May reported 150,376 recovered patients. ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[23] ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[26]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[27] In the latest report (11 September 2020), the number of total deaths is 16,165.[28] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[30]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[30] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[33] ^ GermanyNot all state authorities count recoveries.[44]Recoveries include estimations by the Robert Koch Institute.[44][45] ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[50] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[51] ^ RomaniaOn 18 September 2020, the large increase in the number of recoveries was a result of "the review and updating of data by the Ministry of Health and CNCCI".[57] ^ EgyptIncludes cases identified on the MS River Anuket. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[66] ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[69] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[73] ^ ChinaExcluding 366 asymptomatic cases under medical observation as of 17 September 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ MoldovaIncluding the disputed territory of Transnistria. ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[143] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[144] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[155] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[156] ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomaliaExcluding the de facto state of Somaliland. ^ Some of these deaths may still be under investigation as stated in the Ministry's press release. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana1,350 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[229] ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[238] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[239][240][241] ^ SomalilandCases from this de facto state are not counted by Somalia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ TaiwanIncluding cases from the ROCS Pan Shi.[257] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[268] ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[309][310]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[313]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[319]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[320][321] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[325] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[326][327]</t>
+          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reported to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations. ^ Deaths: Reporting criteria vary between locations. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations and some countries do not report recoveries. ^ The worldwide totals for cases, deaths and recoveries are taken from the John Hopkins University Coronavirus Resource Center. They are not sums of the figures for the listed countries and territories. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ SpainThe figure for cases excludes serology–confirmed cases.As of 19 May 2020, the Spanish government does not publish the number of recoveries. The last update on 18 May reported 150,376 recovered patients. ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[23] ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[26]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[27] In the latest report (11 September 2020), the number of total deaths is 16,165.[28] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[30]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[30] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[34] ^ GermanyNot all state authorities count recoveries.[45]Recoveries include estimations by the Robert Koch Institute.[45][46] ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[51] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[52] ^ RomaniaOn 18 September 2020, the large increase in the number of recoveries was a result of "the review and updating of data by the Ministry of Health and CNCCI".[58] ^ EgyptIncludes cases identified on the MS River Anuket. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[67] ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[70] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[73] ^ ChinaExcluding 374 asymptomatic cases under medical observation as of 18 September 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ MoldovaIncluding the disputed territory of Transnistria. ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[144] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[145] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[156] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[157] ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomaliaExcluding the de facto state of Somaliland. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ Some of these deaths may still be under investigation as stated in the Ministry's press release. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana1,350 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[231] ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[240] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[241][242][243] ^ SomalilandCases from this de facto state are not counted by Somalia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ TaiwanIncluding cases from the ROCS Pan Shi.[259] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[270] ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[311][312]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[315]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[321]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[322][323] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[327] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[328][329]</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
         <is>
-          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reported to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations. ^ Deaths: Reporting criteria vary between locations. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations and some countries do not report recoveries. ^ The worldwide totals for cases, deaths and recoveries are taken from the John Hopkins University Coronavirus Resource Center. They are not sums of the figures for the listed countries and territories. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ SpainThe figure for cases excludes serology–confirmed cases.As of 19 May 2020, the Spanish government does not publish the number of recoveries. The last update on 18 May reported 150,376 recovered patients. ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[23] ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[26]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[27] In the latest report (11 September 2020), the number of total deaths is 16,165.[28] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[30]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[30] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[33] ^ GermanyNot all state authorities count recoveries.[44]Recoveries include estimations by the Robert Koch Institute.[44][45] ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[50] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[51] ^ RomaniaOn 18 September 2020, the large increase in the number of recoveries was a result of "the review and updating of data by the Ministry of Health and CNCCI".[57] ^ EgyptIncludes cases identified on the MS River Anuket. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[66] ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[69] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[73] ^ ChinaExcluding 366 asymptomatic cases under medical observation as of 17 September 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ MoldovaIncluding the disputed territory of Transnistria. ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[143] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[144] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[155] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[156] ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomaliaExcluding the de facto state of Somaliland. ^ Some of these deaths may still be under investigation as stated in the Ministry's press release. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana1,350 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[229] ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[238] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[239][240][241] ^ SomalilandCases from this de facto state are not counted by Somalia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ TaiwanIncluding cases from the ROCS Pan Shi.[257] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[268] ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[309][310]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[313]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[319]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[320][321] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[325] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[326][327]</t>
+          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reported to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations. ^ Deaths: Reporting criteria vary between locations. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations and some countries do not report recoveries. ^ The worldwide totals for cases, deaths and recoveries are taken from the John Hopkins University Coronavirus Resource Center. They are not sums of the figures for the listed countries and territories. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ SpainThe figure for cases excludes serology–confirmed cases.As of 19 May 2020, the Spanish government does not publish the number of recoveries. The last update on 18 May reported 150,376 recovered patients. ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[23] ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[26]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[27] In the latest report (11 September 2020), the number of total deaths is 16,165.[28] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[30]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[30] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[34] ^ GermanyNot all state authorities count recoveries.[45]Recoveries include estimations by the Robert Koch Institute.[45][46] ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[51] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[52] ^ RomaniaOn 18 September 2020, the large increase in the number of recoveries was a result of "the review and updating of data by the Ministry of Health and CNCCI".[58] ^ EgyptIncludes cases identified on the MS River Anuket. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[67] ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[70] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[73] ^ ChinaExcluding 374 asymptomatic cases under medical observation as of 18 September 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ MoldovaIncluding the disputed territory of Transnistria. ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[144] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[145] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[156] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[157] ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomaliaExcluding the de facto state of Somaliland. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ Some of these deaths may still be under investigation as stated in the Ministry's press release. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana1,350 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[231] ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[240] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[241][242][243] ^ SomalilandCases from this de facto state are not counted by Somalia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ TaiwanIncluding cases from the ROCS Pan Shi.[259] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[270] ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[311][312]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[315]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[321]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[322][323] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[327] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[328][329]</t>
         </is>
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reported to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations. ^ Deaths: Reporting criteria vary between locations. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations and some countries do not report recoveries. ^ The worldwide totals for cases, deaths and recoveries are taken from the John Hopkins University Coronavirus Resource Center. They are not sums of the figures for the listed countries and territories. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ SpainThe figure for cases excludes serology–confirmed cases.As of 19 May 2020, the Spanish government does not publish the number of recoveries. The last update on 18 May reported 150,376 recovered patients. ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[23] ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[26]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[27] In the latest report (11 September 2020), the number of total deaths is 16,165.[28] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[30]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[30] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[33] ^ GermanyNot all state authorities count recoveries.[44]Recoveries include estimations by the Robert Koch Institute.[44][45] ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[50] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[51] ^ RomaniaOn 18 September 2020, the large increase in the number of recoveries was a result of "the review and updating of data by the Ministry of Health and CNCCI".[57] ^ EgyptIncludes cases identified on the MS River Anuket. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[66] ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[69] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[73] ^ ChinaExcluding 366 asymptomatic cases under medical observation as of 17 September 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ MoldovaIncluding the disputed territory of Transnistria. ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[143] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[144] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[155] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[156] ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomaliaExcluding the de facto state of Somaliland. ^ Some of these deaths may still be under investigation as stated in the Ministry's press release. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana1,350 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[229] ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[238] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[239][240][241] ^ SomalilandCases from this de facto state are not counted by Somalia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ TaiwanIncluding cases from the ROCS Pan Shi.[257] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[268] ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[309][310]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[313]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[319]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[320][321] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[325] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[326][327]</t>
+          <t>Notes ^ Location: Countries, territories, and international conveyances where cases were diagnosed. The nationality of the infected and the origin of infection may vary. For some countries, cases are split into respective territories and noted accordingly. ^ Cases: This number shows the cumulative number of confirmed human cases reported to date. The actual number of infections and cases is likely to be higher than reported.[1] Reporting criteria and testing capacity vary between locations. ^ Deaths: Reporting criteria vary between locations. ^ Recoveries: May not correspond to actual current figures and not all recoveries may be reported. Reporting criteria vary between locations and some countries do not report recoveries. ^ The worldwide totals for cases, deaths and recoveries are taken from the John Hopkins University Coronavirus Resource Center. They are not sums of the figures for the listed countries and territories. ^ United StatesFigures include cases identified on the Grand Princess.Figures do not include the unincorporated territories of Puerto Rico, Guam, Northern Mariana Islands, and U.S. Virgin Islands, all of which are listed separately.Not all states or overseas territories report recovery data.Cases include clinically diagnosed cases as per CDC guidelines.[3]Recoveries and deaths include probable deaths and people released from quarantine as per CDC guidelines.[4][5][6]Figures from the United States Department of Defense are only released on a branch-by branch basis since April 2020, without distinction between domestic and foreign deployment, and cases may be reported to local health authorities.[7]Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separate from national figures but included in the Navy's totals.There is also one case reported from Guantanamo Bay Naval Base not included in any other nation or territory's counts.[8] Since April 2020, the United States Department of Defense has directed all bases, including Guantanamo Bay, to not publish case statistics.[7] ^ BrazilSince 6 June, the Brazilian government has ordered the Ministry of Health to stop reporting the total number of deaths and active cases.[11] After this, the National Council of Health Secretaries assumed the function of reporting the total number of deaths and active cases.[12] ^ RussiaIncluding cases from the disputed Crimea and Sevastopol.Excluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". ^ SpainThe figure for cases excludes serology–confirmed cases.As of 19 May 2020, the Spanish government does not publish the number of recoveries. The last update on 18 May reported 150,376 recovered patients. ^ ArgentinaExcluding confirmed cases on the claimed territory of the Falkland Islands. Since 11 April, the Argentine Ministry of Health includes them in their official reports.[23] ^ Chile Including the special territory of Easter Island.The Chilean Ministry of Health considered all cases as "recovered" after 14 days since the initial symptoms of the virus, no matter the health situation of the infected or if following tests indicate the continuing presence of the virus. The only exception were casualties, which are not included as recovered.[26]Deaths only include cases with positive PCR tests and catalogued as "COVID-19 related death" by the Civil Registry and Identification Service. This number is informed on the daily reports of the Ministry of Health. A report with the total number of deaths, including suspected cases without PCR test, is released weekly since 20 June 2020.[27] In the latest report (11 September 2020), the number of total deaths is 16,165.[28] ^ FranceIncluding overseas regions of French Guiana, Guadeloupe, Martinique, Mayotte and Réunion, and collectivities of Saint Barthélemy and Saint Martin.Excluding collectivities of New Caledonia, French Polynesia and Saint Pierre and Miquelon.Recoveries only include hospitalized cases.[30]Figures for total confirmed cases and total deaths include data from both hospital and nursing home (ESMS: établissements sociaux et médico-sociaux).[30] ^ United KingdomExcluding all British Overseas Territories and Crown dependencies.As of 23 March 2020, the UK government does not publish the number of recoveries. The last update on 22 March reported 135 recovered patients.[34] ^ GermanyNot all state authorities count recoveries.[45]Recoveries include estimations by the Robert Koch Institute.[45][46] ^ IsraelIncluding cases from the disputed Golan Heights.Excluding cases from the Occupied Palestinian Territories. ^ UkraineExcluding cases from the disputed Crimea and Sevastopol. Cases in these territories are included in the Russian total.Excluding cases from the unrecognized Donetsk and Lugansk People's Republics. ^ Canada On 17 July 2020, Quebec, Canada, revised its criteria on recoveries. The Institut national de santé publique claims that "the previous method resulted in 'significant underestimations' of recovered cases."[51] This change resulted in a drop of active cases nationwide, from a total of 27,603 on 16 July to 4,058 on 17 July.[52] ^ RomaniaOn 18 September 2020, the large increase in the number of recoveries was a result of "the review and updating of data by the Ministry of Health and CNCCI".[58] ^ EgyptIncludes cases identified on the MS River Anuket. ^ BelgiumThe number of deaths also includes untested cases and cases in retirement homes that presumably died because of COVID-19, whilst most countries only include deaths of tested cases in hospitals.[67] ^ MoroccoIncluding cases in the disputed Western Sahara territory controlled by Morocco. There are no confirmed cases in the rest of Western Sahara.[70] ^ NetherlandsThe Kingdom of the Netherlands consists of a) the Netherlands* [the country as opposed to the kingdom; listed here], which in turn includes the Caribbean Netherlands, that are made up of the special municipalities Bonaire*, Saba* and Sint Eustatius*; b) Aruba*; c) Curaçao*; and d) Sint Maarten*. All regions marked with an asterisk are listed separately.The Dutch Government agency RIVM, responsible for the constituent country the Netherlands, does not count its number of recoveries.[73] ^ ChinaExcluding 374 asymptomatic cases under medical observation as of 18 September 2020Asymptomatic cases were not reported before 31 March 2020.Excluding Special Administrative Regions of Hong Kong and Macau.Does not include Taiwan. ^ a b Diamond Princess and JapanThe British cruise ship Diamond Princess was in Japanese waters, and the Japanese administration was asked to manage its quarantine, with the passengers having not entered Japan. Therefore, this case is included in neither the Japanese nor British official counts. The World Health Organization classifies the cases as being located "on an international conveyance". ^ SwitzerlandRecoveries are estimates by the Tribune de Genève. ^ MoldovaIncluding the disputed territory of Transnistria. ^ AzerbaijanExcluding the self-declared state of Artsakh. ^ SerbiaExcluding cases from the disputed territory of Kosovo. ^ AustraliaExcluding the cases from Diamond Princess cruise ship which are classified as "on an international conveyance". Ten cases, including one fatality recorded by the Australian government. ^ DenmarkThe autonomous territories of the Faroe Islands and Greenland are listed separately. ^ NorwayEstimation of the number of infected: As of 23 March 2020, according to figures from just over 40 per cent of all GPs in Norway, 20,200 patients have been registered with the "corona code" R991. The figure includes both cases where the patient has been diagnosed with coronavirus infection through testing, and where the GP has used the "corona code" after assessing the patient's symptoms against the criteria by the Norwegian Institute of Public Health.[144] As of 24 March 2020, the Norwegian Institute of Public Health estimates that between 7,120 and 23,140 Norwegians are infected with the coronavirus.[145] ^ DR CongoThe Democratic Republic of the Congo. ^ FinlandIncluding the autonomous region of the Åland Islands.The number of recoveries is an estimate based on reported cases which were reported at least two weeks ago and there is no other monitoring data on the course of the disease.[156] The exact number of recoveries is not known, as only a small proportion of patients have been hospitalized.[157] ^ CubaIncludes cases on the MS Braemar.Excluding cases from Guantanamo Bay, which is governed by the United States. ^ CongoAlso known as the Republic of the Congo and not to be confused with the DR Congo. ^ SyriaExcluding cases from the disputed Golan Heights. ^ SomaliaExcluding the de facto state of Somaliland. ^ GeorgiaExcluding the de facto states of Abkhazia and South Ossetia. ^ Some of these deaths may still be under investigation as stated in the Ministry's press release. ^ a b Donetsk and Luhansk People's RepublicNote that these territories are distinct from the Ukraine-administered regions of the Donetsk and Luhansk Oblasts. ^ a b Guam and USS Theodore Roosevelt Cases for the USS Theodore Roosevelt, currently docked at Guam, are reported separately. ^ a b Greg Mortimer and UruguayAlthough currently anchored off the coast of Uruguay, cases for the Greg Mortimer are currently reported separately. Six have been transferred inland for hospitalization. ^ CyprusIncluding the British Overseas Territory of Akrotiri and Dhekelia.Excluding de facto state of Northern Cyprus. ^ Botswana1,350 people who tested positive have been voluntarily repatriated to their respective countries and are not part of the confirmed case count as a result the Government of Botswana does not include the transferred-out cases.[231] ^ Charles de GaulleIncluding cases on the escort frigate Chevalier Paul.Florence Parly, Minister of the Armed Forces, reported to the National Assembly's National Defense and Armed Forces Committee [fr] that 2010 sailors of the carrier battle group led by Charles de Gaulle had been tested, with 1081 tests returning positive so far.[240] Many of these cases were aboard Charles de Gaulle, some of the cases were reportedly aboard French frigate Chevalier Paul, and it is unclear if any other ships in the battle group had cases on board.[241][242][243] ^ SomalilandCases from this de facto state are not counted by Somalia. ^ AbkhaziaCases from this de facto state are not counted by Georgia. ^ Northern CyprusCases from this de facto state are not counted by Cyprus. ^ TaiwanIncluding cases from the ROCS Pan Shi.[259] ^ ArtsakhCases from this de facto state are not counted by Azerbaijan. ^ Isle of ManRecoveries are presumed. Defined as "An individual testing positive for coronavirus who completes the 14 day self-isolation period from the onset of symptoms who is at home on day 15, or an individual who is discharged from hospital following more severe symptoms."[270] ^ South OssetiaCases from this de facto state are not counted by Georgia. ^ Saint VincentThe sovereign state of Saint Vincent and the Grenadines. ^ MS ZaandamIncluding cases from MS Rotterdam.The MS Rotterdam rendezvoused with the Zaandam on 26 March off the coast of Panama City to provide support and evacuate healthy passengers. Both have since docked in Florida.[311][312]MS Zaandam and Rotterdam's numbers are currently not counted in any national figures. ^ Coral PrincessThe cruise ship Coral Princess has tested positive cases since early April 2020 and has since docked in Miami.[315]Coral Princess's numbers are currently not counted in any national figures. ^ HNLMS Dolfijn All 8 cases currently associated with Dolfijn were reported while the submarine was at sea in the waters between Scotland and the Netherlands.[321]It is unclear whether the National Institute for Public Health and the Environment (RIVM) is including these cases in their total count, but neither their daily update details nor their daily epidemiological situation reports appear to have mentioned the ship, with a breakdown of cases listing the twelve provinces of the country of the Netherlands (as opposed to the kingdom) accounting for all the cases in the total count.[322][323] ^ TanzaniaFigures for Tanzania are "No data" as the country stopped publishing figures on coronavirus cases on 29 April.[327] Figures as of that date were 509 cases, 21 deaths, and 183 recoveries.[328][329]</t>
         </is>
       </c>
     </row>

</xml_diff>